<commit_message>
Update Pathway Evidence type.xlsx
</commit_message>
<xml_diff>
--- a/working_files/Pathway Evidence type.xlsx
+++ b/working_files/Pathway Evidence type.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Documents\GitHub\knetgraphs-gene-traits\working files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Documents\GitHub\knetgraphs-gene-traits\working_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E4B5E5-CCF5-4C8C-A185-68AE1B8D66DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307A682C-06A7-4EF5-B0F1-A72C5F435A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,7 +224,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,18 +251,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF93C47D"/>
         <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -286,11 +280,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -308,16 +311,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -334,6 +334,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +558,7 @@
   <dimension ref="A1:K994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -689,25 +695,25 @@
       <c r="D4" s="6">
         <v>0</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="32">
         <v>2339</v>
       </c>
       <c r="G4" s="8">
         <v>56081</v>
       </c>
-      <c r="H4" s="14">
-        <v>0</v>
-      </c>
-      <c r="I4" s="14">
-        <v>0</v>
-      </c>
-      <c r="J4" s="14">
-        <v>0</v>
-      </c>
-      <c r="K4" s="14">
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
         <v>0</v>
       </c>
     </row>
@@ -730,19 +736,19 @@
       <c r="F5" s="7">
         <v>14732</v>
       </c>
-      <c r="G5" s="14">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="14">
-        <v>0</v>
-      </c>
-      <c r="J5" s="14">
-        <v>0</v>
-      </c>
-      <c r="K5" s="14">
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0</v>
+      </c>
+      <c r="K5" s="13">
         <v>0</v>
       </c>
     </row>
@@ -765,19 +771,19 @@
       <c r="F6" s="7">
         <v>290458</v>
       </c>
-      <c r="G6" s="14">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="14">
-        <v>0</v>
-      </c>
-      <c r="J6" s="14">
-        <v>0</v>
-      </c>
-      <c r="K6" s="14">
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="13">
         <v>0</v>
       </c>
     </row>
@@ -797,22 +803,22 @@
       <c r="E7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>0</v>
       </c>
       <c r="G7" s="8">
         <v>2356</v>
       </c>
-      <c r="H7" s="14">
-        <v>0</v>
-      </c>
-      <c r="I7" s="14">
-        <v>0</v>
-      </c>
-      <c r="J7" s="14">
-        <v>0</v>
-      </c>
-      <c r="K7" s="14">
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0</v>
+      </c>
+      <c r="K7" s="13">
         <v>0</v>
       </c>
     </row>
@@ -832,22 +838,22 @@
       <c r="E8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>0</v>
       </c>
       <c r="G8" s="8">
         <v>40886</v>
       </c>
-      <c r="H8" s="14">
-        <v>0</v>
-      </c>
-      <c r="I8" s="14">
-        <v>0</v>
-      </c>
-      <c r="J8" s="14">
-        <v>0</v>
-      </c>
-      <c r="K8" s="14">
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0</v>
+      </c>
+      <c r="K8" s="13">
         <v>0</v>
       </c>
     </row>
@@ -864,7 +870,7 @@
       <c r="D9" s="10">
         <v>0</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="11">
@@ -905,19 +911,19 @@
       <c r="F10" s="7">
         <v>4239</v>
       </c>
-      <c r="G10" s="14">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14">
-        <v>0</v>
-      </c>
-      <c r="I10" s="14">
-        <v>0</v>
-      </c>
-      <c r="J10" s="14">
-        <v>0</v>
-      </c>
-      <c r="K10" s="14">
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0</v>
+      </c>
+      <c r="K10" s="13">
         <v>0</v>
       </c>
     </row>
@@ -975,19 +981,19 @@
       <c r="F12" s="7">
         <v>81001</v>
       </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0</v>
-      </c>
-      <c r="J12" s="14">
-        <v>0</v>
-      </c>
-      <c r="K12" s="14">
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1042,22 +1048,22 @@
       <c r="E14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <v>0</v>
       </c>
       <c r="G14" s="8">
         <v>1234</v>
       </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="14">
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1112,22 +1118,22 @@
       <c r="E16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <v>0</v>
       </c>
       <c r="G16" s="8">
         <v>47153</v>
       </c>
-      <c r="H16" s="14">
-        <v>0</v>
-      </c>
-      <c r="I16" s="14">
-        <v>0</v>
-      </c>
-      <c r="J16" s="14">
-        <v>0</v>
-      </c>
-      <c r="K16" s="14">
+      <c r="H16" s="13">
+        <v>0</v>
+      </c>
+      <c r="I16" s="13">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+      <c r="K16" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1217,10 +1223,10 @@
       <c r="E19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="15">
-        <v>0</v>
-      </c>
-      <c r="G19" s="14">
+      <c r="F19" s="14">
+        <v>0</v>
+      </c>
+      <c r="G19" s="13">
         <v>0</v>
       </c>
       <c r="H19" s="8">
@@ -1229,10 +1235,10 @@
       <c r="I19" s="8">
         <v>1</v>
       </c>
-      <c r="J19" s="14">
-        <v>0</v>
-      </c>
-      <c r="K19" s="14">
+      <c r="J19" s="13">
+        <v>0</v>
+      </c>
+      <c r="K19" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1290,7 +1296,7 @@
       <c r="F21" s="7">
         <v>9144</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>0</v>
       </c>
       <c r="H21" s="8">
@@ -1325,7 +1331,7 @@
       <c r="F22" s="7">
         <v>183203</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <v>0</v>
       </c>
       <c r="H22" s="8">
@@ -1395,7 +1401,7 @@
       <c r="F24" s="7">
         <v>5027</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <v>0</v>
       </c>
       <c r="H24" s="8">
@@ -1430,7 +1436,7 @@
       <c r="F25" s="7">
         <v>215406</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <v>0</v>
       </c>
       <c r="H25" s="8">
@@ -1447,3233 +1453,3233 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="17"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="20">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19">
         <f t="shared" ref="F27:K27" si="0">SUM(F2:F25)</f>
         <v>1140193</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="18">
         <f t="shared" si="0"/>
         <v>192739</v>
       </c>
-      <c r="H27" s="19">
+      <c r="H27" s="18">
         <f t="shared" si="0"/>
         <v>227534</v>
       </c>
-      <c r="I27" s="19">
+      <c r="I27" s="18">
         <f t="shared" si="0"/>
         <v>307716</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="18">
         <f t="shared" si="0"/>
         <v>257222</v>
       </c>
-      <c r="K27" s="19">
+      <c r="K27" s="18">
         <f t="shared" si="0"/>
         <v>224454</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="26"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="25"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="26"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="25"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="26"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="25"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="26"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="25"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="26"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="25"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="26"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="25"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="26"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="25"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="26"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="25"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="26"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="25"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="26"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="25"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="26"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="25"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="26"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="25"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="26"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="25"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="26"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="25"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="26"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="25"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="25"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="24"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="25"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="24"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="25"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="24"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="28"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="25"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="25"/>
+      <c r="A47" s="22"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="24"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="25"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="24"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="25"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="24"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="25"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="24"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="25"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="24"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="25"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="24"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="25"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="24"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="28"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="25"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="24"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="25"/>
+      <c r="A55" s="22"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="24"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
-      <c r="B56" s="28"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="25"/>
+      <c r="A56" s="22"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="24"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="25"/>
+      <c r="A57" s="22"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="24"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
-      <c r="B58" s="28"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="25"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="24"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="25"/>
+      <c r="A59" s="22"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="24"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="28"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="25"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="24"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="25"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="24"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="24"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="25"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="24"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="25"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="24"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="24"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="26"/>
+      <c r="A64" s="23"/>
+      <c r="B64" s="26"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="25"/>
     </row>
     <row r="65" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="25"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="26"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="25"/>
     </row>
     <row r="66" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="26"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="25"/>
     </row>
     <row r="67" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="26"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="25"/>
     </row>
     <row r="68" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="26"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="25"/>
     </row>
     <row r="69" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="26"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="25"/>
     </row>
     <row r="70" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="26"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="25"/>
     </row>
     <row r="71" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="26"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="25"/>
     </row>
     <row r="72" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="26"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="25"/>
     </row>
     <row r="73" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="26"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="25"/>
     </row>
     <row r="74" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="26"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="25"/>
     </row>
     <row r="75" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="26"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="25"/>
     </row>
     <row r="76" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="26"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="25"/>
     </row>
     <row r="77" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="26"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="25"/>
     </row>
     <row r="78" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="26"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="25"/>
     </row>
     <row r="79" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="26"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="25"/>
     </row>
     <row r="80" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="26"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="25"/>
     </row>
     <row r="81" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="26"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="25"/>
     </row>
     <row r="82" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="26"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="25"/>
     </row>
     <row r="83" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="26"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="25"/>
     </row>
     <row r="84" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="25"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="26"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="25"/>
     </row>
     <row r="85" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="26"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="25"/>
     </row>
     <row r="86" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="26"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="25"/>
     </row>
     <row r="87" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="26"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="25"/>
     </row>
     <row r="88" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="26"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="25"/>
     </row>
     <row r="89" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="26"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="25"/>
     </row>
     <row r="90" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="26"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="25"/>
     </row>
     <row r="91" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="26"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="25"/>
     </row>
     <row r="92" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="26"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="25"/>
     </row>
     <row r="93" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="25"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="26"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="25"/>
     </row>
     <row r="94" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="25"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="26"/>
+      <c r="B94" s="24"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="25"/>
     </row>
     <row r="95" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F95" s="17"/>
+      <c r="F95" s="16"/>
     </row>
     <row r="96" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F96" s="17"/>
+      <c r="F96" s="16"/>
     </row>
     <row r="97" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F97" s="17"/>
+      <c r="F97" s="16"/>
     </row>
     <row r="98" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F98" s="17"/>
+      <c r="F98" s="16"/>
     </row>
     <row r="99" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F99" s="17"/>
+      <c r="F99" s="16"/>
     </row>
     <row r="100" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F100" s="17"/>
+      <c r="F100" s="16"/>
     </row>
     <row r="101" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F101" s="17"/>
+      <c r="F101" s="16"/>
     </row>
     <row r="102" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F102" s="17"/>
+      <c r="F102" s="16"/>
     </row>
     <row r="103" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F103" s="17"/>
+      <c r="F103" s="16"/>
     </row>
     <row r="104" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F104" s="17"/>
+      <c r="F104" s="16"/>
     </row>
     <row r="105" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F105" s="17"/>
+      <c r="F105" s="16"/>
     </row>
     <row r="106" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F106" s="17"/>
+      <c r="F106" s="16"/>
     </row>
     <row r="107" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F107" s="17"/>
+      <c r="F107" s="16"/>
     </row>
     <row r="108" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F108" s="17"/>
+      <c r="F108" s="16"/>
     </row>
     <row r="109" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F109" s="17"/>
+      <c r="F109" s="16"/>
     </row>
     <row r="110" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F110" s="17"/>
+      <c r="F110" s="16"/>
     </row>
     <row r="111" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F111" s="17"/>
+      <c r="F111" s="16"/>
     </row>
     <row r="112" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F112" s="17"/>
+      <c r="F112" s="16"/>
     </row>
     <row r="113" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F113" s="17"/>
+      <c r="F113" s="16"/>
     </row>
     <row r="114" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F114" s="17"/>
+      <c r="F114" s="16"/>
     </row>
     <row r="115" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F115" s="17"/>
+      <c r="F115" s="16"/>
     </row>
     <row r="116" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F116" s="17"/>
+      <c r="F116" s="16"/>
     </row>
     <row r="117" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F117" s="17"/>
+      <c r="F117" s="16"/>
     </row>
     <row r="118" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F118" s="17"/>
+      <c r="F118" s="16"/>
     </row>
     <row r="119" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F119" s="17"/>
+      <c r="F119" s="16"/>
     </row>
     <row r="120" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F120" s="17"/>
+      <c r="F120" s="16"/>
     </row>
     <row r="121" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F121" s="17"/>
+      <c r="F121" s="16"/>
     </row>
     <row r="122" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F122" s="17"/>
+      <c r="F122" s="16"/>
     </row>
     <row r="123" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F123" s="17"/>
+      <c r="F123" s="16"/>
     </row>
     <row r="124" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F124" s="17"/>
+      <c r="F124" s="16"/>
     </row>
     <row r="125" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F125" s="17"/>
+      <c r="F125" s="16"/>
     </row>
     <row r="126" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F126" s="17"/>
+      <c r="F126" s="16"/>
     </row>
     <row r="127" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F127" s="17"/>
+      <c r="F127" s="16"/>
     </row>
     <row r="128" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F128" s="17"/>
+      <c r="F128" s="16"/>
     </row>
     <row r="129" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F129" s="17"/>
+      <c r="F129" s="16"/>
     </row>
     <row r="130" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F130" s="17"/>
+      <c r="F130" s="16"/>
     </row>
     <row r="131" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F131" s="17"/>
+      <c r="F131" s="16"/>
     </row>
     <row r="132" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F132" s="17"/>
+      <c r="F132" s="16"/>
     </row>
     <row r="133" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F133" s="17"/>
+      <c r="F133" s="16"/>
     </row>
     <row r="134" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F134" s="17"/>
+      <c r="F134" s="16"/>
     </row>
     <row r="135" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F135" s="17"/>
+      <c r="F135" s="16"/>
     </row>
     <row r="136" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F136" s="17"/>
+      <c r="F136" s="16"/>
     </row>
     <row r="137" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F137" s="17"/>
+      <c r="F137" s="16"/>
     </row>
     <row r="138" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F138" s="17"/>
+      <c r="F138" s="16"/>
     </row>
     <row r="139" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F139" s="17"/>
+      <c r="F139" s="16"/>
     </row>
     <row r="140" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F140" s="17"/>
+      <c r="F140" s="16"/>
     </row>
     <row r="141" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F141" s="17"/>
+      <c r="F141" s="16"/>
     </row>
     <row r="142" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F142" s="17"/>
+      <c r="F142" s="16"/>
     </row>
     <row r="143" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F143" s="17"/>
+      <c r="F143" s="16"/>
     </row>
     <row r="144" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F144" s="17"/>
+      <c r="F144" s="16"/>
     </row>
     <row r="145" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F145" s="17"/>
+      <c r="F145" s="16"/>
     </row>
     <row r="146" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F146" s="17"/>
+      <c r="F146" s="16"/>
     </row>
     <row r="147" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F147" s="17"/>
+      <c r="F147" s="16"/>
     </row>
     <row r="148" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F148" s="17"/>
+      <c r="F148" s="16"/>
     </row>
     <row r="149" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F149" s="17"/>
+      <c r="F149" s="16"/>
     </row>
     <row r="150" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F150" s="17"/>
+      <c r="F150" s="16"/>
     </row>
     <row r="151" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F151" s="17"/>
+      <c r="F151" s="16"/>
     </row>
     <row r="152" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F152" s="17"/>
+      <c r="F152" s="16"/>
     </row>
     <row r="153" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F153" s="17"/>
+      <c r="F153" s="16"/>
     </row>
     <row r="154" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F154" s="17"/>
+      <c r="F154" s="16"/>
     </row>
     <row r="155" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F155" s="17"/>
+      <c r="F155" s="16"/>
     </row>
     <row r="156" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F156" s="17"/>
+      <c r="F156" s="16"/>
     </row>
     <row r="157" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F157" s="17"/>
+      <c r="F157" s="16"/>
     </row>
     <row r="158" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F158" s="17"/>
+      <c r="F158" s="16"/>
     </row>
     <row r="159" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F159" s="17"/>
+      <c r="F159" s="16"/>
     </row>
     <row r="160" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F160" s="17"/>
+      <c r="F160" s="16"/>
     </row>
     <row r="161" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F161" s="17"/>
+      <c r="F161" s="16"/>
     </row>
     <row r="162" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F162" s="17"/>
+      <c r="F162" s="16"/>
     </row>
     <row r="163" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F163" s="17"/>
+      <c r="F163" s="16"/>
     </row>
     <row r="164" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F164" s="17"/>
+      <c r="F164" s="16"/>
     </row>
     <row r="165" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F165" s="17"/>
+      <c r="F165" s="16"/>
     </row>
     <row r="166" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F166" s="17"/>
+      <c r="F166" s="16"/>
     </row>
     <row r="167" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F167" s="17"/>
+      <c r="F167" s="16"/>
     </row>
     <row r="168" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F168" s="17"/>
+      <c r="F168" s="16"/>
     </row>
     <row r="169" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F169" s="17"/>
+      <c r="F169" s="16"/>
     </row>
     <row r="170" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F170" s="17"/>
+      <c r="F170" s="16"/>
     </row>
     <row r="171" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F171" s="17"/>
+      <c r="F171" s="16"/>
     </row>
     <row r="172" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F172" s="17"/>
+      <c r="F172" s="16"/>
     </row>
     <row r="173" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F173" s="17"/>
+      <c r="F173" s="16"/>
     </row>
     <row r="174" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F174" s="17"/>
+      <c r="F174" s="16"/>
     </row>
     <row r="175" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F175" s="17"/>
+      <c r="F175" s="16"/>
     </row>
     <row r="176" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F176" s="17"/>
+      <c r="F176" s="16"/>
     </row>
     <row r="177" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F177" s="17"/>
+      <c r="F177" s="16"/>
     </row>
     <row r="178" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F178" s="17"/>
+      <c r="F178" s="16"/>
     </row>
     <row r="179" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F179" s="17"/>
+      <c r="F179" s="16"/>
     </row>
     <row r="180" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F180" s="17"/>
+      <c r="F180" s="16"/>
     </row>
     <row r="181" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F181" s="17"/>
+      <c r="F181" s="16"/>
     </row>
     <row r="182" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F182" s="17"/>
+      <c r="F182" s="16"/>
     </row>
     <row r="183" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F183" s="17"/>
+      <c r="F183" s="16"/>
     </row>
     <row r="184" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F184" s="17"/>
+      <c r="F184" s="16"/>
     </row>
     <row r="185" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F185" s="17"/>
+      <c r="F185" s="16"/>
     </row>
     <row r="186" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F186" s="17"/>
+      <c r="F186" s="16"/>
     </row>
     <row r="187" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F187" s="17"/>
+      <c r="F187" s="16"/>
     </row>
     <row r="188" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F188" s="17"/>
+      <c r="F188" s="16"/>
     </row>
     <row r="189" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F189" s="17"/>
+      <c r="F189" s="16"/>
     </row>
     <row r="190" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F190" s="17"/>
+      <c r="F190" s="16"/>
     </row>
     <row r="191" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F191" s="17"/>
+      <c r="F191" s="16"/>
     </row>
     <row r="192" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F192" s="17"/>
+      <c r="F192" s="16"/>
     </row>
     <row r="193" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F193" s="17"/>
+      <c r="F193" s="16"/>
     </row>
     <row r="194" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F194" s="17"/>
+      <c r="F194" s="16"/>
     </row>
     <row r="195" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F195" s="17"/>
+      <c r="F195" s="16"/>
     </row>
     <row r="196" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F196" s="17"/>
+      <c r="F196" s="16"/>
     </row>
     <row r="197" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F197" s="17"/>
+      <c r="F197" s="16"/>
     </row>
     <row r="198" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F198" s="17"/>
+      <c r="F198" s="16"/>
     </row>
     <row r="199" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F199" s="17"/>
+      <c r="F199" s="16"/>
     </row>
     <row r="200" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F200" s="17"/>
+      <c r="F200" s="16"/>
     </row>
     <row r="201" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F201" s="17"/>
+      <c r="F201" s="16"/>
     </row>
     <row r="202" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F202" s="17"/>
+      <c r="F202" s="16"/>
     </row>
     <row r="203" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F203" s="17"/>
+      <c r="F203" s="16"/>
     </row>
     <row r="204" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F204" s="17"/>
+      <c r="F204" s="16"/>
     </row>
     <row r="205" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F205" s="17"/>
+      <c r="F205" s="16"/>
     </row>
     <row r="206" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F206" s="17"/>
+      <c r="F206" s="16"/>
     </row>
     <row r="207" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F207" s="17"/>
+      <c r="F207" s="16"/>
     </row>
     <row r="208" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F208" s="17"/>
+      <c r="F208" s="16"/>
     </row>
     <row r="209" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F209" s="17"/>
+      <c r="F209" s="16"/>
     </row>
     <row r="210" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F210" s="17"/>
+      <c r="F210" s="16"/>
     </row>
     <row r="211" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F211" s="17"/>
+      <c r="F211" s="16"/>
     </row>
     <row r="212" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F212" s="17"/>
+      <c r="F212" s="16"/>
     </row>
     <row r="213" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F213" s="17"/>
+      <c r="F213" s="16"/>
     </row>
     <row r="214" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F214" s="17"/>
+      <c r="F214" s="16"/>
     </row>
     <row r="215" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F215" s="17"/>
+      <c r="F215" s="16"/>
     </row>
     <row r="216" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F216" s="17"/>
+      <c r="F216" s="16"/>
     </row>
     <row r="217" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F217" s="17"/>
+      <c r="F217" s="16"/>
     </row>
     <row r="218" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F218" s="17"/>
+      <c r="F218" s="16"/>
     </row>
     <row r="219" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F219" s="17"/>
+      <c r="F219" s="16"/>
     </row>
     <row r="220" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F220" s="17"/>
+      <c r="F220" s="16"/>
     </row>
     <row r="221" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F221" s="17"/>
+      <c r="F221" s="16"/>
     </row>
     <row r="222" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F222" s="17"/>
+      <c r="F222" s="16"/>
     </row>
     <row r="223" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F223" s="17"/>
+      <c r="F223" s="16"/>
     </row>
     <row r="224" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F224" s="17"/>
+      <c r="F224" s="16"/>
     </row>
     <row r="225" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F225" s="17"/>
+      <c r="F225" s="16"/>
     </row>
     <row r="226" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F226" s="17"/>
+      <c r="F226" s="16"/>
     </row>
     <row r="227" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F227" s="17"/>
+      <c r="F227" s="16"/>
     </row>
     <row r="228" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F228" s="17"/>
+      <c r="F228" s="16"/>
     </row>
     <row r="229" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F229" s="17"/>
+      <c r="F229" s="16"/>
     </row>
     <row r="230" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F230" s="17"/>
+      <c r="F230" s="16"/>
     </row>
     <row r="231" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F231" s="17"/>
+      <c r="F231" s="16"/>
     </row>
     <row r="232" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F232" s="17"/>
+      <c r="F232" s="16"/>
     </row>
     <row r="233" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F233" s="17"/>
+      <c r="F233" s="16"/>
     </row>
     <row r="234" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F234" s="17"/>
+      <c r="F234" s="16"/>
     </row>
     <row r="235" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F235" s="17"/>
+      <c r="F235" s="16"/>
     </row>
     <row r="236" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F236" s="17"/>
+      <c r="F236" s="16"/>
     </row>
     <row r="237" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F237" s="17"/>
+      <c r="F237" s="16"/>
     </row>
     <row r="238" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F238" s="17"/>
+      <c r="F238" s="16"/>
     </row>
     <row r="239" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F239" s="17"/>
+      <c r="F239" s="16"/>
     </row>
     <row r="240" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F240" s="17"/>
+      <c r="F240" s="16"/>
     </row>
     <row r="241" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F241" s="17"/>
+      <c r="F241" s="16"/>
     </row>
     <row r="242" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F242" s="17"/>
+      <c r="F242" s="16"/>
     </row>
     <row r="243" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F243" s="17"/>
+      <c r="F243" s="16"/>
     </row>
     <row r="244" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F244" s="17"/>
+      <c r="F244" s="16"/>
     </row>
     <row r="245" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F245" s="17"/>
+      <c r="F245" s="16"/>
     </row>
     <row r="246" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F246" s="17"/>
+      <c r="F246" s="16"/>
     </row>
     <row r="247" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F247" s="17"/>
+      <c r="F247" s="16"/>
     </row>
     <row r="248" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F248" s="17"/>
+      <c r="F248" s="16"/>
     </row>
     <row r="249" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F249" s="17"/>
+      <c r="F249" s="16"/>
     </row>
     <row r="250" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F250" s="17"/>
+      <c r="F250" s="16"/>
     </row>
     <row r="251" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F251" s="17"/>
+      <c r="F251" s="16"/>
     </row>
     <row r="252" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F252" s="17"/>
+      <c r="F252" s="16"/>
     </row>
     <row r="253" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F253" s="17"/>
+      <c r="F253" s="16"/>
     </row>
     <row r="254" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F254" s="17"/>
+      <c r="F254" s="16"/>
     </row>
     <row r="255" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F255" s="17"/>
+      <c r="F255" s="16"/>
     </row>
     <row r="256" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F256" s="17"/>
+      <c r="F256" s="16"/>
     </row>
     <row r="257" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F257" s="17"/>
+      <c r="F257" s="16"/>
     </row>
     <row r="258" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F258" s="17"/>
+      <c r="F258" s="16"/>
     </row>
     <row r="259" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F259" s="17"/>
+      <c r="F259" s="16"/>
     </row>
     <row r="260" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F260" s="17"/>
+      <c r="F260" s="16"/>
     </row>
     <row r="261" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F261" s="17"/>
+      <c r="F261" s="16"/>
     </row>
     <row r="262" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F262" s="17"/>
+      <c r="F262" s="16"/>
     </row>
     <row r="263" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F263" s="17"/>
+      <c r="F263" s="16"/>
     </row>
     <row r="264" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F264" s="17"/>
+      <c r="F264" s="16"/>
     </row>
     <row r="265" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F265" s="17"/>
+      <c r="F265" s="16"/>
     </row>
     <row r="266" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F266" s="17"/>
+      <c r="F266" s="16"/>
     </row>
     <row r="267" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F267" s="17"/>
+      <c r="F267" s="16"/>
     </row>
     <row r="268" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F268" s="17"/>
+      <c r="F268" s="16"/>
     </row>
     <row r="269" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F269" s="17"/>
+      <c r="F269" s="16"/>
     </row>
     <row r="270" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F270" s="17"/>
+      <c r="F270" s="16"/>
     </row>
     <row r="271" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F271" s="17"/>
+      <c r="F271" s="16"/>
     </row>
     <row r="272" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F272" s="17"/>
+      <c r="F272" s="16"/>
     </row>
     <row r="273" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F273" s="17"/>
+      <c r="F273" s="16"/>
     </row>
     <row r="274" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F274" s="17"/>
+      <c r="F274" s="16"/>
     </row>
     <row r="275" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F275" s="17"/>
+      <c r="F275" s="16"/>
     </row>
     <row r="276" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F276" s="17"/>
+      <c r="F276" s="16"/>
     </row>
     <row r="277" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F277" s="17"/>
+      <c r="F277" s="16"/>
     </row>
     <row r="278" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F278" s="17"/>
+      <c r="F278" s="16"/>
     </row>
     <row r="279" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F279" s="17"/>
+      <c r="F279" s="16"/>
     </row>
     <row r="280" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F280" s="17"/>
+      <c r="F280" s="16"/>
     </row>
     <row r="281" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F281" s="17"/>
+      <c r="F281" s="16"/>
     </row>
     <row r="282" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F282" s="17"/>
+      <c r="F282" s="16"/>
     </row>
     <row r="283" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F283" s="17"/>
+      <c r="F283" s="16"/>
     </row>
     <row r="284" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F284" s="17"/>
+      <c r="F284" s="16"/>
     </row>
     <row r="285" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F285" s="17"/>
+      <c r="F285" s="16"/>
     </row>
     <row r="286" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F286" s="17"/>
+      <c r="F286" s="16"/>
     </row>
     <row r="287" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F287" s="17"/>
+      <c r="F287" s="16"/>
     </row>
     <row r="288" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F288" s="17"/>
+      <c r="F288" s="16"/>
     </row>
     <row r="289" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F289" s="17"/>
+      <c r="F289" s="16"/>
     </row>
     <row r="290" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F290" s="17"/>
+      <c r="F290" s="16"/>
     </row>
     <row r="291" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F291" s="17"/>
+      <c r="F291" s="16"/>
     </row>
     <row r="292" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F292" s="17"/>
+      <c r="F292" s="16"/>
     </row>
     <row r="293" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F293" s="17"/>
+      <c r="F293" s="16"/>
     </row>
     <row r="294" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F294" s="17"/>
+      <c r="F294" s="16"/>
     </row>
     <row r="295" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F295" s="17"/>
+      <c r="F295" s="16"/>
     </row>
     <row r="296" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F296" s="17"/>
+      <c r="F296" s="16"/>
     </row>
     <row r="297" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F297" s="17"/>
+      <c r="F297" s="16"/>
     </row>
     <row r="298" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F298" s="17"/>
+      <c r="F298" s="16"/>
     </row>
     <row r="299" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F299" s="17"/>
+      <c r="F299" s="16"/>
     </row>
     <row r="300" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F300" s="17"/>
+      <c r="F300" s="16"/>
     </row>
     <row r="301" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F301" s="17"/>
+      <c r="F301" s="16"/>
     </row>
     <row r="302" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F302" s="17"/>
+      <c r="F302" s="16"/>
     </row>
     <row r="303" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F303" s="17"/>
+      <c r="F303" s="16"/>
     </row>
     <row r="304" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F304" s="17"/>
+      <c r="F304" s="16"/>
     </row>
     <row r="305" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F305" s="17"/>
+      <c r="F305" s="16"/>
     </row>
     <row r="306" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F306" s="17"/>
+      <c r="F306" s="16"/>
     </row>
     <row r="307" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F307" s="17"/>
+      <c r="F307" s="16"/>
     </row>
     <row r="308" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F308" s="17"/>
+      <c r="F308" s="16"/>
     </row>
     <row r="309" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F309" s="17"/>
+      <c r="F309" s="16"/>
     </row>
     <row r="310" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F310" s="17"/>
+      <c r="F310" s="16"/>
     </row>
     <row r="311" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F311" s="17"/>
+      <c r="F311" s="16"/>
     </row>
     <row r="312" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F312" s="17"/>
+      <c r="F312" s="16"/>
     </row>
     <row r="313" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F313" s="17"/>
+      <c r="F313" s="16"/>
     </row>
     <row r="314" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F314" s="17"/>
+      <c r="F314" s="16"/>
     </row>
     <row r="315" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F315" s="17"/>
+      <c r="F315" s="16"/>
     </row>
     <row r="316" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F316" s="17"/>
+      <c r="F316" s="16"/>
     </row>
     <row r="317" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F317" s="17"/>
+      <c r="F317" s="16"/>
     </row>
     <row r="318" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F318" s="17"/>
+      <c r="F318" s="16"/>
     </row>
     <row r="319" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F319" s="17"/>
+      <c r="F319" s="16"/>
     </row>
     <row r="320" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F320" s="17"/>
+      <c r="F320" s="16"/>
     </row>
     <row r="321" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F321" s="17"/>
+      <c r="F321" s="16"/>
     </row>
     <row r="322" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F322" s="17"/>
+      <c r="F322" s="16"/>
     </row>
     <row r="323" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F323" s="17"/>
+      <c r="F323" s="16"/>
     </row>
     <row r="324" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F324" s="17"/>
+      <c r="F324" s="16"/>
     </row>
     <row r="325" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F325" s="17"/>
+      <c r="F325" s="16"/>
     </row>
     <row r="326" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F326" s="17"/>
+      <c r="F326" s="16"/>
     </row>
     <row r="327" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F327" s="17"/>
+      <c r="F327" s="16"/>
     </row>
     <row r="328" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F328" s="17"/>
+      <c r="F328" s="16"/>
     </row>
     <row r="329" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F329" s="17"/>
+      <c r="F329" s="16"/>
     </row>
     <row r="330" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F330" s="17"/>
+      <c r="F330" s="16"/>
     </row>
     <row r="331" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F331" s="17"/>
+      <c r="F331" s="16"/>
     </row>
     <row r="332" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F332" s="17"/>
+      <c r="F332" s="16"/>
     </row>
     <row r="333" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F333" s="17"/>
+      <c r="F333" s="16"/>
     </row>
     <row r="334" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F334" s="17"/>
+      <c r="F334" s="16"/>
     </row>
     <row r="335" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F335" s="17"/>
+      <c r="F335" s="16"/>
     </row>
     <row r="336" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F336" s="17"/>
+      <c r="F336" s="16"/>
     </row>
     <row r="337" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F337" s="17"/>
+      <c r="F337" s="16"/>
     </row>
     <row r="338" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F338" s="17"/>
+      <c r="F338" s="16"/>
     </row>
     <row r="339" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F339" s="17"/>
+      <c r="F339" s="16"/>
     </row>
     <row r="340" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F340" s="17"/>
+      <c r="F340" s="16"/>
     </row>
     <row r="341" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F341" s="17"/>
+      <c r="F341" s="16"/>
     </row>
     <row r="342" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F342" s="17"/>
+      <c r="F342" s="16"/>
     </row>
     <row r="343" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F343" s="17"/>
+      <c r="F343" s="16"/>
     </row>
     <row r="344" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F344" s="17"/>
+      <c r="F344" s="16"/>
     </row>
     <row r="345" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F345" s="17"/>
+      <c r="F345" s="16"/>
     </row>
     <row r="346" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F346" s="17"/>
+      <c r="F346" s="16"/>
     </row>
     <row r="347" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F347" s="17"/>
+      <c r="F347" s="16"/>
     </row>
     <row r="348" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F348" s="17"/>
+      <c r="F348" s="16"/>
     </row>
     <row r="349" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F349" s="17"/>
+      <c r="F349" s="16"/>
     </row>
     <row r="350" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F350" s="17"/>
+      <c r="F350" s="16"/>
     </row>
     <row r="351" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F351" s="17"/>
+      <c r="F351" s="16"/>
     </row>
     <row r="352" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F352" s="17"/>
+      <c r="F352" s="16"/>
     </row>
     <row r="353" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F353" s="17"/>
+      <c r="F353" s="16"/>
     </row>
     <row r="354" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F354" s="17"/>
+      <c r="F354" s="16"/>
     </row>
     <row r="355" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F355" s="17"/>
+      <c r="F355" s="16"/>
     </row>
     <row r="356" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F356" s="17"/>
+      <c r="F356" s="16"/>
     </row>
     <row r="357" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F357" s="17"/>
+      <c r="F357" s="16"/>
     </row>
     <row r="358" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F358" s="17"/>
+      <c r="F358" s="16"/>
     </row>
     <row r="359" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F359" s="17"/>
+      <c r="F359" s="16"/>
     </row>
     <row r="360" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F360" s="17"/>
+      <c r="F360" s="16"/>
     </row>
     <row r="361" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F361" s="17"/>
+      <c r="F361" s="16"/>
     </row>
     <row r="362" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F362" s="17"/>
+      <c r="F362" s="16"/>
     </row>
     <row r="363" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F363" s="17"/>
+      <c r="F363" s="16"/>
     </row>
     <row r="364" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F364" s="17"/>
+      <c r="F364" s="16"/>
     </row>
     <row r="365" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F365" s="17"/>
+      <c r="F365" s="16"/>
     </row>
     <row r="366" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F366" s="17"/>
+      <c r="F366" s="16"/>
     </row>
     <row r="367" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F367" s="17"/>
+      <c r="F367" s="16"/>
     </row>
     <row r="368" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F368" s="17"/>
+      <c r="F368" s="16"/>
     </row>
     <row r="369" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F369" s="17"/>
+      <c r="F369" s="16"/>
     </row>
     <row r="370" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F370" s="17"/>
+      <c r="F370" s="16"/>
     </row>
     <row r="371" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F371" s="17"/>
+      <c r="F371" s="16"/>
     </row>
     <row r="372" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F372" s="17"/>
+      <c r="F372" s="16"/>
     </row>
     <row r="373" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F373" s="17"/>
+      <c r="F373" s="16"/>
     </row>
     <row r="374" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F374" s="17"/>
+      <c r="F374" s="16"/>
     </row>
     <row r="375" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F375" s="17"/>
+      <c r="F375" s="16"/>
     </row>
     <row r="376" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F376" s="17"/>
+      <c r="F376" s="16"/>
     </row>
     <row r="377" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F377" s="17"/>
+      <c r="F377" s="16"/>
     </row>
     <row r="378" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F378" s="17"/>
+      <c r="F378" s="16"/>
     </row>
     <row r="379" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F379" s="17"/>
+      <c r="F379" s="16"/>
     </row>
     <row r="380" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F380" s="17"/>
+      <c r="F380" s="16"/>
     </row>
     <row r="381" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F381" s="17"/>
+      <c r="F381" s="16"/>
     </row>
     <row r="382" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F382" s="17"/>
+      <c r="F382" s="16"/>
     </row>
     <row r="383" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F383" s="17"/>
+      <c r="F383" s="16"/>
     </row>
     <row r="384" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F384" s="17"/>
+      <c r="F384" s="16"/>
     </row>
     <row r="385" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F385" s="17"/>
+      <c r="F385" s="16"/>
     </row>
     <row r="386" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F386" s="17"/>
+      <c r="F386" s="16"/>
     </row>
     <row r="387" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F387" s="17"/>
+      <c r="F387" s="16"/>
     </row>
     <row r="388" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F388" s="17"/>
+      <c r="F388" s="16"/>
     </row>
     <row r="389" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F389" s="17"/>
+      <c r="F389" s="16"/>
     </row>
     <row r="390" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F390" s="17"/>
+      <c r="F390" s="16"/>
     </row>
     <row r="391" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F391" s="17"/>
+      <c r="F391" s="16"/>
     </row>
     <row r="392" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F392" s="17"/>
+      <c r="F392" s="16"/>
     </row>
     <row r="393" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F393" s="17"/>
+      <c r="F393" s="16"/>
     </row>
     <row r="394" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F394" s="17"/>
+      <c r="F394" s="16"/>
     </row>
     <row r="395" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F395" s="17"/>
+      <c r="F395" s="16"/>
     </row>
     <row r="396" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F396" s="17"/>
+      <c r="F396" s="16"/>
     </row>
     <row r="397" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F397" s="17"/>
+      <c r="F397" s="16"/>
     </row>
     <row r="398" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F398" s="17"/>
+      <c r="F398" s="16"/>
     </row>
     <row r="399" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F399" s="17"/>
+      <c r="F399" s="16"/>
     </row>
     <row r="400" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F400" s="17"/>
+      <c r="F400" s="16"/>
     </row>
     <row r="401" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F401" s="17"/>
+      <c r="F401" s="16"/>
     </row>
     <row r="402" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F402" s="17"/>
+      <c r="F402" s="16"/>
     </row>
     <row r="403" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F403" s="17"/>
+      <c r="F403" s="16"/>
     </row>
     <row r="404" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F404" s="17"/>
+      <c r="F404" s="16"/>
     </row>
     <row r="405" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F405" s="17"/>
+      <c r="F405" s="16"/>
     </row>
     <row r="406" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F406" s="17"/>
+      <c r="F406" s="16"/>
     </row>
     <row r="407" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F407" s="17"/>
+      <c r="F407" s="16"/>
     </row>
     <row r="408" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F408" s="17"/>
+      <c r="F408" s="16"/>
     </row>
     <row r="409" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F409" s="17"/>
+      <c r="F409" s="16"/>
     </row>
     <row r="410" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F410" s="17"/>
+      <c r="F410" s="16"/>
     </row>
     <row r="411" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F411" s="17"/>
+      <c r="F411" s="16"/>
     </row>
     <row r="412" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F412" s="17"/>
+      <c r="F412" s="16"/>
     </row>
     <row r="413" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F413" s="17"/>
+      <c r="F413" s="16"/>
     </row>
     <row r="414" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F414" s="17"/>
+      <c r="F414" s="16"/>
     </row>
     <row r="415" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F415" s="17"/>
+      <c r="F415" s="16"/>
     </row>
     <row r="416" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F416" s="17"/>
+      <c r="F416" s="16"/>
     </row>
     <row r="417" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F417" s="17"/>
+      <c r="F417" s="16"/>
     </row>
     <row r="418" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F418" s="17"/>
+      <c r="F418" s="16"/>
     </row>
     <row r="419" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F419" s="17"/>
+      <c r="F419" s="16"/>
     </row>
     <row r="420" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F420" s="17"/>
+      <c r="F420" s="16"/>
     </row>
     <row r="421" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F421" s="17"/>
+      <c r="F421" s="16"/>
     </row>
     <row r="422" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F422" s="17"/>
+      <c r="F422" s="16"/>
     </row>
     <row r="423" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F423" s="17"/>
+      <c r="F423" s="16"/>
     </row>
     <row r="424" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F424" s="17"/>
+      <c r="F424" s="16"/>
     </row>
     <row r="425" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F425" s="17"/>
+      <c r="F425" s="16"/>
     </row>
     <row r="426" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F426" s="17"/>
+      <c r="F426" s="16"/>
     </row>
     <row r="427" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F427" s="17"/>
+      <c r="F427" s="16"/>
     </row>
     <row r="428" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F428" s="17"/>
+      <c r="F428" s="16"/>
     </row>
     <row r="429" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F429" s="17"/>
+      <c r="F429" s="16"/>
     </row>
     <row r="430" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F430" s="17"/>
+      <c r="F430" s="16"/>
     </row>
     <row r="431" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F431" s="17"/>
+      <c r="F431" s="16"/>
     </row>
     <row r="432" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F432" s="17"/>
+      <c r="F432" s="16"/>
     </row>
     <row r="433" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F433" s="17"/>
+      <c r="F433" s="16"/>
     </row>
     <row r="434" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F434" s="17"/>
+      <c r="F434" s="16"/>
     </row>
     <row r="435" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F435" s="17"/>
+      <c r="F435" s="16"/>
     </row>
     <row r="436" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F436" s="17"/>
+      <c r="F436" s="16"/>
     </row>
     <row r="437" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F437" s="17"/>
+      <c r="F437" s="16"/>
     </row>
     <row r="438" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F438" s="17"/>
+      <c r="F438" s="16"/>
     </row>
     <row r="439" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F439" s="17"/>
+      <c r="F439" s="16"/>
     </row>
     <row r="440" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F440" s="17"/>
+      <c r="F440" s="16"/>
     </row>
     <row r="441" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F441" s="17"/>
+      <c r="F441" s="16"/>
     </row>
     <row r="442" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F442" s="17"/>
+      <c r="F442" s="16"/>
     </row>
     <row r="443" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F443" s="17"/>
+      <c r="F443" s="16"/>
     </row>
     <row r="444" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F444" s="17"/>
+      <c r="F444" s="16"/>
     </row>
     <row r="445" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F445" s="17"/>
+      <c r="F445" s="16"/>
     </row>
     <row r="446" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F446" s="17"/>
+      <c r="F446" s="16"/>
     </row>
     <row r="447" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F447" s="17"/>
+      <c r="F447" s="16"/>
     </row>
     <row r="448" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F448" s="17"/>
+      <c r="F448" s="16"/>
     </row>
     <row r="449" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F449" s="17"/>
+      <c r="F449" s="16"/>
     </row>
     <row r="450" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F450" s="17"/>
+      <c r="F450" s="16"/>
     </row>
     <row r="451" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F451" s="17"/>
+      <c r="F451" s="16"/>
     </row>
     <row r="452" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F452" s="17"/>
+      <c r="F452" s="16"/>
     </row>
     <row r="453" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F453" s="17"/>
+      <c r="F453" s="16"/>
     </row>
     <row r="454" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F454" s="17"/>
+      <c r="F454" s="16"/>
     </row>
     <row r="455" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F455" s="17"/>
+      <c r="F455" s="16"/>
     </row>
     <row r="456" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F456" s="17"/>
+      <c r="F456" s="16"/>
     </row>
     <row r="457" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F457" s="17"/>
+      <c r="F457" s="16"/>
     </row>
     <row r="458" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F458" s="17"/>
+      <c r="F458" s="16"/>
     </row>
     <row r="459" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F459" s="17"/>
+      <c r="F459" s="16"/>
     </row>
     <row r="460" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F460" s="17"/>
+      <c r="F460" s="16"/>
     </row>
     <row r="461" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F461" s="17"/>
+      <c r="F461" s="16"/>
     </row>
     <row r="462" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F462" s="17"/>
+      <c r="F462" s="16"/>
     </row>
     <row r="463" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F463" s="17"/>
+      <c r="F463" s="16"/>
     </row>
     <row r="464" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F464" s="17"/>
+      <c r="F464" s="16"/>
     </row>
     <row r="465" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F465" s="17"/>
+      <c r="F465" s="16"/>
     </row>
     <row r="466" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F466" s="17"/>
+      <c r="F466" s="16"/>
     </row>
     <row r="467" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F467" s="17"/>
+      <c r="F467" s="16"/>
     </row>
     <row r="468" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F468" s="17"/>
+      <c r="F468" s="16"/>
     </row>
     <row r="469" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F469" s="17"/>
+      <c r="F469" s="16"/>
     </row>
     <row r="470" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F470" s="17"/>
+      <c r="F470" s="16"/>
     </row>
     <row r="471" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F471" s="17"/>
+      <c r="F471" s="16"/>
     </row>
     <row r="472" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F472" s="17"/>
+      <c r="F472" s="16"/>
     </row>
     <row r="473" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F473" s="17"/>
+      <c r="F473" s="16"/>
     </row>
     <row r="474" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F474" s="17"/>
+      <c r="F474" s="16"/>
     </row>
     <row r="475" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F475" s="17"/>
+      <c r="F475" s="16"/>
     </row>
     <row r="476" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F476" s="17"/>
+      <c r="F476" s="16"/>
     </row>
     <row r="477" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F477" s="17"/>
+      <c r="F477" s="16"/>
     </row>
     <row r="478" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F478" s="17"/>
+      <c r="F478" s="16"/>
     </row>
     <row r="479" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F479" s="17"/>
+      <c r="F479" s="16"/>
     </row>
     <row r="480" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F480" s="17"/>
+      <c r="F480" s="16"/>
     </row>
     <row r="481" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F481" s="17"/>
+      <c r="F481" s="16"/>
     </row>
     <row r="482" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F482" s="17"/>
+      <c r="F482" s="16"/>
     </row>
     <row r="483" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F483" s="17"/>
+      <c r="F483" s="16"/>
     </row>
     <row r="484" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F484" s="17"/>
+      <c r="F484" s="16"/>
     </row>
     <row r="485" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F485" s="17"/>
+      <c r="F485" s="16"/>
     </row>
     <row r="486" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F486" s="17"/>
+      <c r="F486" s="16"/>
     </row>
     <row r="487" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F487" s="17"/>
+      <c r="F487" s="16"/>
     </row>
     <row r="488" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F488" s="17"/>
+      <c r="F488" s="16"/>
     </row>
     <row r="489" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F489" s="17"/>
+      <c r="F489" s="16"/>
     </row>
     <row r="490" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F490" s="17"/>
+      <c r="F490" s="16"/>
     </row>
     <row r="491" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F491" s="17"/>
+      <c r="F491" s="16"/>
     </row>
     <row r="492" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F492" s="17"/>
+      <c r="F492" s="16"/>
     </row>
     <row r="493" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F493" s="17"/>
+      <c r="F493" s="16"/>
     </row>
     <row r="494" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F494" s="17"/>
+      <c r="F494" s="16"/>
     </row>
     <row r="495" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F495" s="17"/>
+      <c r="F495" s="16"/>
     </row>
     <row r="496" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F496" s="17"/>
+      <c r="F496" s="16"/>
     </row>
     <row r="497" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F497" s="17"/>
+      <c r="F497" s="16"/>
     </row>
     <row r="498" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F498" s="17"/>
+      <c r="F498" s="16"/>
     </row>
     <row r="499" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F499" s="17"/>
+      <c r="F499" s="16"/>
     </row>
     <row r="500" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F500" s="17"/>
+      <c r="F500" s="16"/>
     </row>
     <row r="501" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F501" s="17"/>
+      <c r="F501" s="16"/>
     </row>
     <row r="502" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F502" s="17"/>
+      <c r="F502" s="16"/>
     </row>
     <row r="503" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F503" s="17"/>
+      <c r="F503" s="16"/>
     </row>
     <row r="504" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F504" s="17"/>
+      <c r="F504" s="16"/>
     </row>
     <row r="505" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F505" s="17"/>
+      <c r="F505" s="16"/>
     </row>
     <row r="506" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F506" s="17"/>
+      <c r="F506" s="16"/>
     </row>
     <row r="507" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F507" s="17"/>
+      <c r="F507" s="16"/>
     </row>
     <row r="508" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F508" s="17"/>
+      <c r="F508" s="16"/>
     </row>
     <row r="509" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F509" s="17"/>
+      <c r="F509" s="16"/>
     </row>
     <row r="510" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F510" s="17"/>
+      <c r="F510" s="16"/>
     </row>
     <row r="511" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F511" s="17"/>
+      <c r="F511" s="16"/>
     </row>
     <row r="512" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F512" s="17"/>
+      <c r="F512" s="16"/>
     </row>
     <row r="513" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F513" s="17"/>
+      <c r="F513" s="16"/>
     </row>
     <row r="514" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F514" s="17"/>
+      <c r="F514" s="16"/>
     </row>
     <row r="515" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F515" s="17"/>
+      <c r="F515" s="16"/>
     </row>
     <row r="516" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F516" s="17"/>
+      <c r="F516" s="16"/>
     </row>
     <row r="517" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F517" s="17"/>
+      <c r="F517" s="16"/>
     </row>
     <row r="518" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F518" s="17"/>
+      <c r="F518" s="16"/>
     </row>
     <row r="519" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F519" s="17"/>
+      <c r="F519" s="16"/>
     </row>
     <row r="520" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F520" s="17"/>
+      <c r="F520" s="16"/>
     </row>
     <row r="521" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F521" s="17"/>
+      <c r="F521" s="16"/>
     </row>
     <row r="522" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F522" s="17"/>
+      <c r="F522" s="16"/>
     </row>
     <row r="523" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F523" s="17"/>
+      <c r="F523" s="16"/>
     </row>
     <row r="524" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F524" s="17"/>
+      <c r="F524" s="16"/>
     </row>
     <row r="525" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F525" s="17"/>
+      <c r="F525" s="16"/>
     </row>
     <row r="526" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F526" s="17"/>
+      <c r="F526" s="16"/>
     </row>
     <row r="527" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F527" s="17"/>
+      <c r="F527" s="16"/>
     </row>
     <row r="528" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F528" s="17"/>
+      <c r="F528" s="16"/>
     </row>
     <row r="529" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F529" s="17"/>
+      <c r="F529" s="16"/>
     </row>
     <row r="530" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F530" s="17"/>
+      <c r="F530" s="16"/>
     </row>
     <row r="531" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F531" s="17"/>
+      <c r="F531" s="16"/>
     </row>
     <row r="532" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F532" s="17"/>
+      <c r="F532" s="16"/>
     </row>
     <row r="533" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F533" s="17"/>
+      <c r="F533" s="16"/>
     </row>
     <row r="534" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F534" s="17"/>
+      <c r="F534" s="16"/>
     </row>
     <row r="535" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F535" s="17"/>
+      <c r="F535" s="16"/>
     </row>
     <row r="536" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F536" s="17"/>
+      <c r="F536" s="16"/>
     </row>
     <row r="537" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F537" s="17"/>
+      <c r="F537" s="16"/>
     </row>
     <row r="538" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F538" s="17"/>
+      <c r="F538" s="16"/>
     </row>
     <row r="539" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F539" s="17"/>
+      <c r="F539" s="16"/>
     </row>
     <row r="540" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F540" s="17"/>
+      <c r="F540" s="16"/>
     </row>
     <row r="541" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F541" s="17"/>
+      <c r="F541" s="16"/>
     </row>
     <row r="542" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F542" s="17"/>
+      <c r="F542" s="16"/>
     </row>
     <row r="543" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F543" s="17"/>
+      <c r="F543" s="16"/>
     </row>
     <row r="544" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F544" s="17"/>
+      <c r="F544" s="16"/>
     </row>
     <row r="545" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F545" s="17"/>
+      <c r="F545" s="16"/>
     </row>
     <row r="546" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F546" s="17"/>
+      <c r="F546" s="16"/>
     </row>
     <row r="547" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F547" s="17"/>
+      <c r="F547" s="16"/>
     </row>
     <row r="548" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F548" s="17"/>
+      <c r="F548" s="16"/>
     </row>
     <row r="549" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F549" s="17"/>
+      <c r="F549" s="16"/>
     </row>
     <row r="550" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F550" s="17"/>
+      <c r="F550" s="16"/>
     </row>
     <row r="551" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F551" s="17"/>
+      <c r="F551" s="16"/>
     </row>
     <row r="552" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F552" s="17"/>
+      <c r="F552" s="16"/>
     </row>
     <row r="553" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F553" s="17"/>
+      <c r="F553" s="16"/>
     </row>
     <row r="554" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F554" s="17"/>
+      <c r="F554" s="16"/>
     </row>
     <row r="555" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F555" s="17"/>
+      <c r="F555" s="16"/>
     </row>
     <row r="556" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F556" s="17"/>
+      <c r="F556" s="16"/>
     </row>
     <row r="557" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F557" s="17"/>
+      <c r="F557" s="16"/>
     </row>
     <row r="558" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F558" s="17"/>
+      <c r="F558" s="16"/>
     </row>
     <row r="559" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F559" s="17"/>
+      <c r="F559" s="16"/>
     </row>
     <row r="560" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F560" s="17"/>
+      <c r="F560" s="16"/>
     </row>
     <row r="561" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F561" s="17"/>
+      <c r="F561" s="16"/>
     </row>
     <row r="562" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F562" s="17"/>
+      <c r="F562" s="16"/>
     </row>
     <row r="563" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F563" s="17"/>
+      <c r="F563" s="16"/>
     </row>
     <row r="564" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F564" s="17"/>
+      <c r="F564" s="16"/>
     </row>
     <row r="565" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F565" s="17"/>
+      <c r="F565" s="16"/>
     </row>
     <row r="566" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F566" s="17"/>
+      <c r="F566" s="16"/>
     </row>
     <row r="567" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F567" s="17"/>
+      <c r="F567" s="16"/>
     </row>
     <row r="568" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F568" s="17"/>
+      <c r="F568" s="16"/>
     </row>
     <row r="569" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F569" s="17"/>
+      <c r="F569" s="16"/>
     </row>
     <row r="570" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F570" s="17"/>
+      <c r="F570" s="16"/>
     </row>
     <row r="571" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F571" s="17"/>
+      <c r="F571" s="16"/>
     </row>
     <row r="572" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F572" s="17"/>
+      <c r="F572" s="16"/>
     </row>
     <row r="573" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F573" s="17"/>
+      <c r="F573" s="16"/>
     </row>
     <row r="574" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F574" s="17"/>
+      <c r="F574" s="16"/>
     </row>
     <row r="575" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F575" s="17"/>
+      <c r="F575" s="16"/>
     </row>
     <row r="576" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F576" s="17"/>
+      <c r="F576" s="16"/>
     </row>
     <row r="577" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F577" s="17"/>
+      <c r="F577" s="16"/>
     </row>
     <row r="578" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F578" s="17"/>
+      <c r="F578" s="16"/>
     </row>
     <row r="579" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F579" s="17"/>
+      <c r="F579" s="16"/>
     </row>
     <row r="580" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F580" s="17"/>
+      <c r="F580" s="16"/>
     </row>
     <row r="581" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F581" s="17"/>
+      <c r="F581" s="16"/>
     </row>
     <row r="582" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F582" s="17"/>
+      <c r="F582" s="16"/>
     </row>
     <row r="583" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F583" s="17"/>
+      <c r="F583" s="16"/>
     </row>
     <row r="584" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F584" s="17"/>
+      <c r="F584" s="16"/>
     </row>
     <row r="585" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F585" s="17"/>
+      <c r="F585" s="16"/>
     </row>
     <row r="586" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F586" s="17"/>
+      <c r="F586" s="16"/>
     </row>
     <row r="587" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F587" s="17"/>
+      <c r="F587" s="16"/>
     </row>
     <row r="588" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F588" s="17"/>
+      <c r="F588" s="16"/>
     </row>
     <row r="589" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F589" s="17"/>
+      <c r="F589" s="16"/>
     </row>
     <row r="590" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F590" s="17"/>
+      <c r="F590" s="16"/>
     </row>
     <row r="591" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F591" s="17"/>
+      <c r="F591" s="16"/>
     </row>
     <row r="592" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F592" s="17"/>
+      <c r="F592" s="16"/>
     </row>
     <row r="593" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F593" s="17"/>
+      <c r="F593" s="16"/>
     </row>
     <row r="594" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F594" s="17"/>
+      <c r="F594" s="16"/>
     </row>
     <row r="595" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F595" s="17"/>
+      <c r="F595" s="16"/>
     </row>
     <row r="596" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F596" s="17"/>
+      <c r="F596" s="16"/>
     </row>
     <row r="597" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F597" s="17"/>
+      <c r="F597" s="16"/>
     </row>
     <row r="598" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F598" s="17"/>
+      <c r="F598" s="16"/>
     </row>
     <row r="599" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F599" s="17"/>
+      <c r="F599" s="16"/>
     </row>
     <row r="600" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F600" s="17"/>
+      <c r="F600" s="16"/>
     </row>
     <row r="601" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F601" s="17"/>
+      <c r="F601" s="16"/>
     </row>
     <row r="602" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F602" s="17"/>
+      <c r="F602" s="16"/>
     </row>
     <row r="603" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F603" s="17"/>
+      <c r="F603" s="16"/>
     </row>
     <row r="604" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F604" s="17"/>
+      <c r="F604" s="16"/>
     </row>
     <row r="605" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F605" s="17"/>
+      <c r="F605" s="16"/>
     </row>
     <row r="606" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F606" s="17"/>
+      <c r="F606" s="16"/>
     </row>
     <row r="607" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F607" s="17"/>
+      <c r="F607" s="16"/>
     </row>
     <row r="608" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F608" s="17"/>
+      <c r="F608" s="16"/>
     </row>
     <row r="609" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F609" s="17"/>
+      <c r="F609" s="16"/>
     </row>
     <row r="610" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F610" s="17"/>
+      <c r="F610" s="16"/>
     </row>
     <row r="611" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F611" s="17"/>
+      <c r="F611" s="16"/>
     </row>
     <row r="612" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F612" s="17"/>
+      <c r="F612" s="16"/>
     </row>
     <row r="613" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F613" s="17"/>
+      <c r="F613" s="16"/>
     </row>
     <row r="614" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F614" s="17"/>
+      <c r="F614" s="16"/>
     </row>
     <row r="615" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F615" s="17"/>
+      <c r="F615" s="16"/>
     </row>
     <row r="616" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F616" s="17"/>
+      <c r="F616" s="16"/>
     </row>
     <row r="617" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F617" s="17"/>
+      <c r="F617" s="16"/>
     </row>
     <row r="618" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F618" s="17"/>
+      <c r="F618" s="16"/>
     </row>
     <row r="619" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F619" s="17"/>
+      <c r="F619" s="16"/>
     </row>
     <row r="620" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F620" s="17"/>
+      <c r="F620" s="16"/>
     </row>
     <row r="621" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F621" s="17"/>
+      <c r="F621" s="16"/>
     </row>
     <row r="622" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F622" s="17"/>
+      <c r="F622" s="16"/>
     </row>
     <row r="623" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F623" s="17"/>
+      <c r="F623" s="16"/>
     </row>
     <row r="624" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F624" s="17"/>
+      <c r="F624" s="16"/>
     </row>
     <row r="625" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F625" s="17"/>
+      <c r="F625" s="16"/>
     </row>
     <row r="626" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F626" s="17"/>
+      <c r="F626" s="16"/>
     </row>
     <row r="627" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F627" s="17"/>
+      <c r="F627" s="16"/>
     </row>
     <row r="628" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F628" s="17"/>
+      <c r="F628" s="16"/>
     </row>
     <row r="629" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F629" s="17"/>
+      <c r="F629" s="16"/>
     </row>
     <row r="630" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F630" s="17"/>
+      <c r="F630" s="16"/>
     </row>
     <row r="631" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F631" s="17"/>
+      <c r="F631" s="16"/>
     </row>
     <row r="632" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F632" s="17"/>
+      <c r="F632" s="16"/>
     </row>
     <row r="633" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F633" s="17"/>
+      <c r="F633" s="16"/>
     </row>
     <row r="634" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F634" s="17"/>
+      <c r="F634" s="16"/>
     </row>
     <row r="635" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F635" s="17"/>
+      <c r="F635" s="16"/>
     </row>
     <row r="636" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F636" s="17"/>
+      <c r="F636" s="16"/>
     </row>
     <row r="637" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F637" s="17"/>
+      <c r="F637" s="16"/>
     </row>
     <row r="638" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F638" s="17"/>
+      <c r="F638" s="16"/>
     </row>
     <row r="639" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F639" s="17"/>
+      <c r="F639" s="16"/>
     </row>
     <row r="640" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F640" s="17"/>
+      <c r="F640" s="16"/>
     </row>
     <row r="641" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F641" s="17"/>
+      <c r="F641" s="16"/>
     </row>
     <row r="642" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F642" s="17"/>
+      <c r="F642" s="16"/>
     </row>
     <row r="643" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F643" s="17"/>
+      <c r="F643" s="16"/>
     </row>
     <row r="644" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F644" s="17"/>
+      <c r="F644" s="16"/>
     </row>
     <row r="645" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F645" s="17"/>
+      <c r="F645" s="16"/>
     </row>
     <row r="646" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F646" s="17"/>
+      <c r="F646" s="16"/>
     </row>
     <row r="647" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F647" s="17"/>
+      <c r="F647" s="16"/>
     </row>
     <row r="648" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F648" s="17"/>
+      <c r="F648" s="16"/>
     </row>
     <row r="649" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F649" s="17"/>
+      <c r="F649" s="16"/>
     </row>
     <row r="650" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F650" s="17"/>
+      <c r="F650" s="16"/>
     </row>
     <row r="651" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F651" s="17"/>
+      <c r="F651" s="16"/>
     </row>
     <row r="652" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F652" s="17"/>
+      <c r="F652" s="16"/>
     </row>
     <row r="653" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F653" s="17"/>
+      <c r="F653" s="16"/>
     </row>
     <row r="654" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F654" s="17"/>
+      <c r="F654" s="16"/>
     </row>
     <row r="655" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F655" s="17"/>
+      <c r="F655" s="16"/>
     </row>
     <row r="656" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F656" s="17"/>
+      <c r="F656" s="16"/>
     </row>
     <row r="657" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F657" s="17"/>
+      <c r="F657" s="16"/>
     </row>
     <row r="658" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F658" s="17"/>
+      <c r="F658" s="16"/>
     </row>
     <row r="659" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F659" s="17"/>
+      <c r="F659" s="16"/>
     </row>
     <row r="660" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F660" s="17"/>
+      <c r="F660" s="16"/>
     </row>
     <row r="661" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F661" s="17"/>
+      <c r="F661" s="16"/>
     </row>
     <row r="662" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F662" s="17"/>
+      <c r="F662" s="16"/>
     </row>
     <row r="663" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F663" s="17"/>
+      <c r="F663" s="16"/>
     </row>
     <row r="664" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F664" s="17"/>
+      <c r="F664" s="16"/>
     </row>
     <row r="665" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F665" s="17"/>
+      <c r="F665" s="16"/>
     </row>
     <row r="666" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F666" s="17"/>
+      <c r="F666" s="16"/>
     </row>
     <row r="667" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F667" s="17"/>
+      <c r="F667" s="16"/>
     </row>
     <row r="668" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F668" s="17"/>
+      <c r="F668" s="16"/>
     </row>
     <row r="669" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F669" s="17"/>
+      <c r="F669" s="16"/>
     </row>
     <row r="670" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F670" s="17"/>
+      <c r="F670" s="16"/>
     </row>
     <row r="671" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F671" s="17"/>
+      <c r="F671" s="16"/>
     </row>
     <row r="672" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F672" s="17"/>
+      <c r="F672" s="16"/>
     </row>
     <row r="673" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F673" s="17"/>
+      <c r="F673" s="16"/>
     </row>
     <row r="674" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F674" s="17"/>
+      <c r="F674" s="16"/>
     </row>
     <row r="675" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F675" s="17"/>
+      <c r="F675" s="16"/>
     </row>
     <row r="676" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F676" s="17"/>
+      <c r="F676" s="16"/>
     </row>
     <row r="677" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F677" s="17"/>
+      <c r="F677" s="16"/>
     </row>
     <row r="678" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F678" s="17"/>
+      <c r="F678" s="16"/>
     </row>
     <row r="679" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F679" s="17"/>
+      <c r="F679" s="16"/>
     </row>
     <row r="680" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F680" s="17"/>
+      <c r="F680" s="16"/>
     </row>
     <row r="681" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F681" s="17"/>
+      <c r="F681" s="16"/>
     </row>
     <row r="682" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F682" s="17"/>
+      <c r="F682" s="16"/>
     </row>
     <row r="683" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F683" s="17"/>
+      <c r="F683" s="16"/>
     </row>
     <row r="684" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F684" s="17"/>
+      <c r="F684" s="16"/>
     </row>
     <row r="685" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F685" s="17"/>
+      <c r="F685" s="16"/>
     </row>
     <row r="686" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F686" s="17"/>
+      <c r="F686" s="16"/>
     </row>
     <row r="687" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F687" s="17"/>
+      <c r="F687" s="16"/>
     </row>
     <row r="688" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F688" s="17"/>
+      <c r="F688" s="16"/>
     </row>
     <row r="689" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F689" s="17"/>
+      <c r="F689" s="16"/>
     </row>
     <row r="690" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F690" s="17"/>
+      <c r="F690" s="16"/>
     </row>
     <row r="691" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F691" s="17"/>
+      <c r="F691" s="16"/>
     </row>
     <row r="692" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F692" s="17"/>
+      <c r="F692" s="16"/>
     </row>
     <row r="693" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F693" s="17"/>
+      <c r="F693" s="16"/>
     </row>
     <row r="694" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F694" s="17"/>
+      <c r="F694" s="16"/>
     </row>
     <row r="695" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F695" s="17"/>
+      <c r="F695" s="16"/>
     </row>
     <row r="696" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F696" s="17"/>
+      <c r="F696" s="16"/>
     </row>
     <row r="697" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F697" s="17"/>
+      <c r="F697" s="16"/>
     </row>
     <row r="698" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F698" s="17"/>
+      <c r="F698" s="16"/>
     </row>
     <row r="699" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F699" s="17"/>
+      <c r="F699" s="16"/>
     </row>
     <row r="700" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F700" s="17"/>
+      <c r="F700" s="16"/>
     </row>
     <row r="701" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F701" s="17"/>
+      <c r="F701" s="16"/>
     </row>
     <row r="702" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F702" s="17"/>
+      <c r="F702" s="16"/>
     </row>
     <row r="703" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F703" s="17"/>
+      <c r="F703" s="16"/>
     </row>
     <row r="704" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F704" s="17"/>
+      <c r="F704" s="16"/>
     </row>
     <row r="705" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F705" s="17"/>
+      <c r="F705" s="16"/>
     </row>
     <row r="706" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F706" s="17"/>
+      <c r="F706" s="16"/>
     </row>
     <row r="707" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F707" s="17"/>
+      <c r="F707" s="16"/>
     </row>
     <row r="708" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F708" s="17"/>
+      <c r="F708" s="16"/>
     </row>
     <row r="709" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F709" s="17"/>
+      <c r="F709" s="16"/>
     </row>
     <row r="710" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F710" s="17"/>
+      <c r="F710" s="16"/>
     </row>
     <row r="711" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F711" s="17"/>
+      <c r="F711" s="16"/>
     </row>
     <row r="712" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F712" s="17"/>
+      <c r="F712" s="16"/>
     </row>
     <row r="713" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F713" s="17"/>
+      <c r="F713" s="16"/>
     </row>
     <row r="714" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F714" s="17"/>
+      <c r="F714" s="16"/>
     </row>
     <row r="715" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F715" s="17"/>
+      <c r="F715" s="16"/>
     </row>
     <row r="716" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F716" s="17"/>
+      <c r="F716" s="16"/>
     </row>
     <row r="717" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F717" s="17"/>
+      <c r="F717" s="16"/>
     </row>
     <row r="718" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F718" s="17"/>
+      <c r="F718" s="16"/>
     </row>
     <row r="719" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F719" s="17"/>
+      <c r="F719" s="16"/>
     </row>
     <row r="720" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F720" s="17"/>
+      <c r="F720" s="16"/>
     </row>
     <row r="721" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F721" s="17"/>
+      <c r="F721" s="16"/>
     </row>
     <row r="722" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F722" s="17"/>
+      <c r="F722" s="16"/>
     </row>
     <row r="723" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F723" s="17"/>
+      <c r="F723" s="16"/>
     </row>
     <row r="724" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F724" s="17"/>
+      <c r="F724" s="16"/>
     </row>
     <row r="725" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F725" s="17"/>
+      <c r="F725" s="16"/>
     </row>
     <row r="726" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F726" s="17"/>
+      <c r="F726" s="16"/>
     </row>
     <row r="727" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F727" s="17"/>
+      <c r="F727" s="16"/>
     </row>
     <row r="728" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F728" s="17"/>
+      <c r="F728" s="16"/>
     </row>
     <row r="729" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F729" s="17"/>
+      <c r="F729" s="16"/>
     </row>
     <row r="730" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F730" s="17"/>
+      <c r="F730" s="16"/>
     </row>
     <row r="731" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F731" s="17"/>
+      <c r="F731" s="16"/>
     </row>
     <row r="732" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F732" s="17"/>
+      <c r="F732" s="16"/>
     </row>
     <row r="733" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F733" s="17"/>
+      <c r="F733" s="16"/>
     </row>
     <row r="734" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F734" s="17"/>
+      <c r="F734" s="16"/>
     </row>
     <row r="735" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F735" s="17"/>
+      <c r="F735" s="16"/>
     </row>
     <row r="736" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F736" s="17"/>
+      <c r="F736" s="16"/>
     </row>
     <row r="737" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F737" s="17"/>
+      <c r="F737" s="16"/>
     </row>
     <row r="738" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F738" s="17"/>
+      <c r="F738" s="16"/>
     </row>
     <row r="739" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F739" s="17"/>
+      <c r="F739" s="16"/>
     </row>
     <row r="740" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F740" s="17"/>
+      <c r="F740" s="16"/>
     </row>
     <row r="741" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F741" s="17"/>
+      <c r="F741" s="16"/>
     </row>
     <row r="742" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F742" s="17"/>
+      <c r="F742" s="16"/>
     </row>
     <row r="743" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F743" s="17"/>
+      <c r="F743" s="16"/>
     </row>
     <row r="744" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F744" s="17"/>
+      <c r="F744" s="16"/>
     </row>
     <row r="745" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F745" s="17"/>
+      <c r="F745" s="16"/>
     </row>
     <row r="746" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F746" s="17"/>
+      <c r="F746" s="16"/>
     </row>
     <row r="747" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F747" s="17"/>
+      <c r="F747" s="16"/>
     </row>
     <row r="748" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F748" s="17"/>
+      <c r="F748" s="16"/>
     </row>
     <row r="749" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F749" s="17"/>
+      <c r="F749" s="16"/>
     </row>
     <row r="750" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F750" s="17"/>
+      <c r="F750" s="16"/>
     </row>
     <row r="751" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F751" s="17"/>
+      <c r="F751" s="16"/>
     </row>
     <row r="752" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F752" s="17"/>
+      <c r="F752" s="16"/>
     </row>
     <row r="753" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F753" s="17"/>
+      <c r="F753" s="16"/>
     </row>
     <row r="754" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F754" s="17"/>
+      <c r="F754" s="16"/>
     </row>
     <row r="755" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F755" s="17"/>
+      <c r="F755" s="16"/>
     </row>
     <row r="756" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F756" s="17"/>
+      <c r="F756" s="16"/>
     </row>
     <row r="757" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F757" s="17"/>
+      <c r="F757" s="16"/>
     </row>
     <row r="758" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F758" s="17"/>
+      <c r="F758" s="16"/>
     </row>
     <row r="759" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F759" s="17"/>
+      <c r="F759" s="16"/>
     </row>
     <row r="760" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F760" s="17"/>
+      <c r="F760" s="16"/>
     </row>
     <row r="761" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F761" s="17"/>
+      <c r="F761" s="16"/>
     </row>
     <row r="762" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F762" s="17"/>
+      <c r="F762" s="16"/>
     </row>
     <row r="763" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F763" s="17"/>
+      <c r="F763" s="16"/>
     </row>
     <row r="764" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F764" s="17"/>
+      <c r="F764" s="16"/>
     </row>
     <row r="765" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F765" s="17"/>
+      <c r="F765" s="16"/>
     </row>
     <row r="766" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F766" s="17"/>
+      <c r="F766" s="16"/>
     </row>
     <row r="767" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F767" s="17"/>
+      <c r="F767" s="16"/>
     </row>
     <row r="768" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F768" s="17"/>
+      <c r="F768" s="16"/>
     </row>
     <row r="769" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F769" s="17"/>
+      <c r="F769" s="16"/>
     </row>
     <row r="770" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F770" s="17"/>
+      <c r="F770" s="16"/>
     </row>
     <row r="771" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F771" s="17"/>
+      <c r="F771" s="16"/>
     </row>
     <row r="772" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F772" s="17"/>
+      <c r="F772" s="16"/>
     </row>
     <row r="773" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F773" s="17"/>
+      <c r="F773" s="16"/>
     </row>
     <row r="774" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F774" s="17"/>
+      <c r="F774" s="16"/>
     </row>
     <row r="775" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F775" s="17"/>
+      <c r="F775" s="16"/>
     </row>
     <row r="776" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F776" s="17"/>
+      <c r="F776" s="16"/>
     </row>
     <row r="777" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F777" s="17"/>
+      <c r="F777" s="16"/>
     </row>
     <row r="778" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F778" s="17"/>
+      <c r="F778" s="16"/>
     </row>
     <row r="779" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F779" s="17"/>
+      <c r="F779" s="16"/>
     </row>
     <row r="780" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F780" s="17"/>
+      <c r="F780" s="16"/>
     </row>
     <row r="781" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F781" s="17"/>
+      <c r="F781" s="16"/>
     </row>
     <row r="782" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F782" s="17"/>
+      <c r="F782" s="16"/>
     </row>
     <row r="783" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F783" s="17"/>
+      <c r="F783" s="16"/>
     </row>
     <row r="784" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F784" s="17"/>
+      <c r="F784" s="16"/>
     </row>
     <row r="785" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F785" s="17"/>
+      <c r="F785" s="16"/>
     </row>
     <row r="786" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F786" s="17"/>
+      <c r="F786" s="16"/>
     </row>
     <row r="787" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F787" s="17"/>
+      <c r="F787" s="16"/>
     </row>
     <row r="788" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F788" s="17"/>
+      <c r="F788" s="16"/>
     </row>
     <row r="789" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F789" s="17"/>
+      <c r="F789" s="16"/>
     </row>
     <row r="790" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F790" s="17"/>
+      <c r="F790" s="16"/>
     </row>
     <row r="791" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F791" s="17"/>
+      <c r="F791" s="16"/>
     </row>
     <row r="792" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F792" s="17"/>
+      <c r="F792" s="16"/>
     </row>
     <row r="793" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F793" s="17"/>
+      <c r="F793" s="16"/>
     </row>
     <row r="794" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F794" s="17"/>
+      <c r="F794" s="16"/>
     </row>
     <row r="795" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F795" s="17"/>
+      <c r="F795" s="16"/>
     </row>
     <row r="796" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F796" s="17"/>
+      <c r="F796" s="16"/>
     </row>
     <row r="797" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F797" s="17"/>
+      <c r="F797" s="16"/>
     </row>
     <row r="798" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F798" s="17"/>
+      <c r="F798" s="16"/>
     </row>
     <row r="799" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F799" s="17"/>
+      <c r="F799" s="16"/>
     </row>
     <row r="800" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F800" s="17"/>
+      <c r="F800" s="16"/>
     </row>
     <row r="801" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F801" s="17"/>
+      <c r="F801" s="16"/>
     </row>
     <row r="802" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F802" s="17"/>
+      <c r="F802" s="16"/>
     </row>
     <row r="803" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F803" s="17"/>
+      <c r="F803" s="16"/>
     </row>
     <row r="804" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F804" s="17"/>
+      <c r="F804" s="16"/>
     </row>
     <row r="805" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F805" s="17"/>
+      <c r="F805" s="16"/>
     </row>
     <row r="806" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F806" s="17"/>
+      <c r="F806" s="16"/>
     </row>
     <row r="807" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F807" s="17"/>
+      <c r="F807" s="16"/>
     </row>
     <row r="808" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F808" s="17"/>
+      <c r="F808" s="16"/>
     </row>
     <row r="809" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F809" s="17"/>
+      <c r="F809" s="16"/>
     </row>
     <row r="810" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F810" s="17"/>
+      <c r="F810" s="16"/>
     </row>
     <row r="811" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F811" s="17"/>
+      <c r="F811" s="16"/>
     </row>
     <row r="812" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F812" s="17"/>
+      <c r="F812" s="16"/>
     </row>
     <row r="813" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F813" s="17"/>
+      <c r="F813" s="16"/>
     </row>
     <row r="814" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F814" s="17"/>
+      <c r="F814" s="16"/>
     </row>
     <row r="815" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F815" s="17"/>
+      <c r="F815" s="16"/>
     </row>
     <row r="816" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F816" s="17"/>
+      <c r="F816" s="16"/>
     </row>
     <row r="817" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F817" s="17"/>
+      <c r="F817" s="16"/>
     </row>
     <row r="818" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F818" s="17"/>
+      <c r="F818" s="16"/>
     </row>
     <row r="819" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F819" s="17"/>
+      <c r="F819" s="16"/>
     </row>
     <row r="820" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F820" s="17"/>
+      <c r="F820" s="16"/>
     </row>
     <row r="821" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F821" s="17"/>
+      <c r="F821" s="16"/>
     </row>
     <row r="822" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F822" s="17"/>
+      <c r="F822" s="16"/>
     </row>
     <row r="823" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F823" s="17"/>
+      <c r="F823" s="16"/>
     </row>
     <row r="824" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F824" s="17"/>
+      <c r="F824" s="16"/>
     </row>
     <row r="825" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F825" s="17"/>
+      <c r="F825" s="16"/>
     </row>
     <row r="826" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F826" s="17"/>
+      <c r="F826" s="16"/>
     </row>
     <row r="827" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F827" s="17"/>
+      <c r="F827" s="16"/>
     </row>
     <row r="828" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F828" s="17"/>
+      <c r="F828" s="16"/>
     </row>
     <row r="829" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F829" s="17"/>
+      <c r="F829" s="16"/>
     </row>
     <row r="830" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F830" s="17"/>
+      <c r="F830" s="16"/>
     </row>
     <row r="831" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F831" s="17"/>
+      <c r="F831" s="16"/>
     </row>
     <row r="832" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F832" s="17"/>
+      <c r="F832" s="16"/>
     </row>
     <row r="833" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F833" s="17"/>
+      <c r="F833" s="16"/>
     </row>
     <row r="834" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F834" s="17"/>
+      <c r="F834" s="16"/>
     </row>
     <row r="835" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F835" s="17"/>
+      <c r="F835" s="16"/>
     </row>
     <row r="836" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F836" s="17"/>
+      <c r="F836" s="16"/>
     </row>
     <row r="837" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F837" s="17"/>
+      <c r="F837" s="16"/>
     </row>
     <row r="838" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F838" s="17"/>
+      <c r="F838" s="16"/>
     </row>
     <row r="839" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F839" s="17"/>
+      <c r="F839" s="16"/>
     </row>
     <row r="840" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F840" s="17"/>
+      <c r="F840" s="16"/>
     </row>
     <row r="841" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F841" s="17"/>
+      <c r="F841" s="16"/>
     </row>
     <row r="842" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F842" s="17"/>
+      <c r="F842" s="16"/>
     </row>
     <row r="843" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F843" s="17"/>
+      <c r="F843" s="16"/>
     </row>
     <row r="844" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F844" s="17"/>
+      <c r="F844" s="16"/>
     </row>
     <row r="845" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F845" s="17"/>
+      <c r="F845" s="16"/>
     </row>
     <row r="846" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F846" s="17"/>
+      <c r="F846" s="16"/>
     </row>
     <row r="847" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F847" s="17"/>
+      <c r="F847" s="16"/>
     </row>
     <row r="848" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F848" s="17"/>
+      <c r="F848" s="16"/>
     </row>
     <row r="849" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F849" s="17"/>
+      <c r="F849" s="16"/>
     </row>
     <row r="850" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F850" s="17"/>
+      <c r="F850" s="16"/>
     </row>
     <row r="851" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F851" s="17"/>
+      <c r="F851" s="16"/>
     </row>
     <row r="852" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F852" s="17"/>
+      <c r="F852" s="16"/>
     </row>
     <row r="853" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F853" s="17"/>
+      <c r="F853" s="16"/>
     </row>
     <row r="854" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F854" s="17"/>
+      <c r="F854" s="16"/>
     </row>
     <row r="855" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F855" s="17"/>
+      <c r="F855" s="16"/>
     </row>
     <row r="856" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F856" s="17"/>
+      <c r="F856" s="16"/>
     </row>
     <row r="857" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F857" s="17"/>
+      <c r="F857" s="16"/>
     </row>
     <row r="858" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F858" s="17"/>
+      <c r="F858" s="16"/>
     </row>
     <row r="859" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F859" s="17"/>
+      <c r="F859" s="16"/>
     </row>
     <row r="860" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F860" s="17"/>
+      <c r="F860" s="16"/>
     </row>
     <row r="861" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F861" s="17"/>
+      <c r="F861" s="16"/>
     </row>
     <row r="862" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F862" s="17"/>
+      <c r="F862" s="16"/>
     </row>
     <row r="863" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F863" s="17"/>
+      <c r="F863" s="16"/>
     </row>
     <row r="864" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F864" s="17"/>
+      <c r="F864" s="16"/>
     </row>
     <row r="865" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F865" s="17"/>
+      <c r="F865" s="16"/>
     </row>
     <row r="866" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F866" s="17"/>
+      <c r="F866" s="16"/>
     </row>
     <row r="867" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F867" s="17"/>
+      <c r="F867" s="16"/>
     </row>
     <row r="868" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F868" s="17"/>
+      <c r="F868" s="16"/>
     </row>
     <row r="869" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F869" s="17"/>
+      <c r="F869" s="16"/>
     </row>
     <row r="870" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F870" s="17"/>
+      <c r="F870" s="16"/>
     </row>
     <row r="871" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F871" s="17"/>
+      <c r="F871" s="16"/>
     </row>
     <row r="872" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F872" s="17"/>
+      <c r="F872" s="16"/>
     </row>
     <row r="873" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F873" s="17"/>
+      <c r="F873" s="16"/>
     </row>
     <row r="874" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F874" s="17"/>
+      <c r="F874" s="16"/>
     </row>
     <row r="875" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F875" s="17"/>
+      <c r="F875" s="16"/>
     </row>
     <row r="876" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F876" s="17"/>
+      <c r="F876" s="16"/>
     </row>
     <row r="877" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F877" s="17"/>
+      <c r="F877" s="16"/>
     </row>
     <row r="878" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F878" s="17"/>
+      <c r="F878" s="16"/>
     </row>
     <row r="879" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F879" s="17"/>
+      <c r="F879" s="16"/>
     </row>
     <row r="880" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F880" s="17"/>
+      <c r="F880" s="16"/>
     </row>
     <row r="881" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F881" s="17"/>
+      <c r="F881" s="16"/>
     </row>
     <row r="882" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F882" s="17"/>
+      <c r="F882" s="16"/>
     </row>
     <row r="883" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F883" s="17"/>
+      <c r="F883" s="16"/>
     </row>
     <row r="884" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F884" s="17"/>
+      <c r="F884" s="16"/>
     </row>
     <row r="885" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F885" s="17"/>
+      <c r="F885" s="16"/>
     </row>
     <row r="886" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F886" s="17"/>
+      <c r="F886" s="16"/>
     </row>
     <row r="887" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F887" s="17"/>
+      <c r="F887" s="16"/>
     </row>
     <row r="888" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F888" s="17"/>
+      <c r="F888" s="16"/>
     </row>
     <row r="889" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F889" s="17"/>
+      <c r="F889" s="16"/>
     </row>
     <row r="890" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F890" s="17"/>
+      <c r="F890" s="16"/>
     </row>
     <row r="891" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F891" s="17"/>
+      <c r="F891" s="16"/>
     </row>
     <row r="892" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F892" s="17"/>
+      <c r="F892" s="16"/>
     </row>
     <row r="893" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F893" s="17"/>
+      <c r="F893" s="16"/>
     </row>
     <row r="894" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F894" s="17"/>
+      <c r="F894" s="16"/>
     </row>
     <row r="895" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F895" s="17"/>
+      <c r="F895" s="16"/>
     </row>
     <row r="896" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F896" s="17"/>
+      <c r="F896" s="16"/>
     </row>
     <row r="897" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F897" s="17"/>
+      <c r="F897" s="16"/>
     </row>
     <row r="898" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F898" s="17"/>
+      <c r="F898" s="16"/>
     </row>
     <row r="899" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F899" s="17"/>
+      <c r="F899" s="16"/>
     </row>
     <row r="900" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F900" s="17"/>
+      <c r="F900" s="16"/>
     </row>
     <row r="901" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F901" s="17"/>
+      <c r="F901" s="16"/>
     </row>
     <row r="902" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F902" s="17"/>
+      <c r="F902" s="16"/>
     </row>
     <row r="903" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F903" s="17"/>
+      <c r="F903" s="16"/>
     </row>
     <row r="904" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F904" s="17"/>
+      <c r="F904" s="16"/>
     </row>
     <row r="905" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F905" s="17"/>
+      <c r="F905" s="16"/>
     </row>
     <row r="906" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F906" s="17"/>
+      <c r="F906" s="16"/>
     </row>
     <row r="907" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F907" s="17"/>
+      <c r="F907" s="16"/>
     </row>
     <row r="908" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F908" s="17"/>
+      <c r="F908" s="16"/>
     </row>
     <row r="909" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F909" s="17"/>
+      <c r="F909" s="16"/>
     </row>
     <row r="910" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F910" s="17"/>
+      <c r="F910" s="16"/>
     </row>
     <row r="911" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F911" s="17"/>
+      <c r="F911" s="16"/>
     </row>
     <row r="912" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F912" s="17"/>
+      <c r="F912" s="16"/>
     </row>
     <row r="913" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F913" s="17"/>
+      <c r="F913" s="16"/>
     </row>
     <row r="914" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F914" s="17"/>
+      <c r="F914" s="16"/>
     </row>
     <row r="915" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F915" s="17"/>
+      <c r="F915" s="16"/>
     </row>
     <row r="916" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F916" s="17"/>
+      <c r="F916" s="16"/>
     </row>
     <row r="917" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F917" s="17"/>
+      <c r="F917" s="16"/>
     </row>
     <row r="918" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F918" s="17"/>
+      <c r="F918" s="16"/>
     </row>
     <row r="919" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F919" s="17"/>
+      <c r="F919" s="16"/>
     </row>
     <row r="920" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F920" s="17"/>
+      <c r="F920" s="16"/>
     </row>
     <row r="921" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F921" s="17"/>
+      <c r="F921" s="16"/>
     </row>
     <row r="922" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F922" s="17"/>
+      <c r="F922" s="16"/>
     </row>
     <row r="923" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F923" s="17"/>
+      <c r="F923" s="16"/>
     </row>
     <row r="924" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F924" s="17"/>
+      <c r="F924" s="16"/>
     </row>
     <row r="925" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F925" s="17"/>
+      <c r="F925" s="16"/>
     </row>
     <row r="926" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F926" s="17"/>
+      <c r="F926" s="16"/>
     </row>
     <row r="927" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F927" s="17"/>
+      <c r="F927" s="16"/>
     </row>
     <row r="928" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F928" s="17"/>
+      <c r="F928" s="16"/>
     </row>
     <row r="929" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F929" s="17"/>
+      <c r="F929" s="16"/>
     </row>
     <row r="930" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F930" s="17"/>
+      <c r="F930" s="16"/>
     </row>
     <row r="931" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F931" s="17"/>
+      <c r="F931" s="16"/>
     </row>
     <row r="932" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F932" s="17"/>
+      <c r="F932" s="16"/>
     </row>
     <row r="933" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F933" s="17"/>
+      <c r="F933" s="16"/>
     </row>
     <row r="934" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F934" s="17"/>
+      <c r="F934" s="16"/>
     </row>
     <row r="935" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F935" s="17"/>
+      <c r="F935" s="16"/>
     </row>
     <row r="936" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F936" s="17"/>
+      <c r="F936" s="16"/>
     </row>
     <row r="937" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F937" s="17"/>
+      <c r="F937" s="16"/>
     </row>
     <row r="938" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F938" s="17"/>
+      <c r="F938" s="16"/>
     </row>
     <row r="939" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F939" s="17"/>
+      <c r="F939" s="16"/>
     </row>
     <row r="940" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F940" s="17"/>
+      <c r="F940" s="16"/>
     </row>
     <row r="941" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F941" s="17"/>
+      <c r="F941" s="16"/>
     </row>
     <row r="942" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F942" s="17"/>
+      <c r="F942" s="16"/>
     </row>
     <row r="943" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F943" s="17"/>
+      <c r="F943" s="16"/>
     </row>
     <row r="944" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F944" s="17"/>
+      <c r="F944" s="16"/>
     </row>
     <row r="945" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F945" s="17"/>
+      <c r="F945" s="16"/>
     </row>
     <row r="946" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F946" s="17"/>
+      <c r="F946" s="16"/>
     </row>
     <row r="947" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F947" s="17"/>
+      <c r="F947" s="16"/>
     </row>
     <row r="948" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F948" s="17"/>
+      <c r="F948" s="16"/>
     </row>
     <row r="949" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F949" s="17"/>
+      <c r="F949" s="16"/>
     </row>
     <row r="950" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F950" s="17"/>
+      <c r="F950" s="16"/>
     </row>
     <row r="951" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F951" s="17"/>
+      <c r="F951" s="16"/>
     </row>
     <row r="952" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F952" s="17"/>
+      <c r="F952" s="16"/>
     </row>
     <row r="953" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F953" s="17"/>
+      <c r="F953" s="16"/>
     </row>
     <row r="954" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F954" s="17"/>
+      <c r="F954" s="16"/>
     </row>
     <row r="955" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F955" s="17"/>
+      <c r="F955" s="16"/>
     </row>
     <row r="956" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F956" s="17"/>
+      <c r="F956" s="16"/>
     </row>
     <row r="957" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F957" s="17"/>
+      <c r="F957" s="16"/>
     </row>
     <row r="958" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F958" s="17"/>
+      <c r="F958" s="16"/>
     </row>
     <row r="959" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F959" s="17"/>
+      <c r="F959" s="16"/>
     </row>
     <row r="960" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F960" s="17"/>
+      <c r="F960" s="16"/>
     </row>
     <row r="961" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F961" s="17"/>
+      <c r="F961" s="16"/>
     </row>
     <row r="962" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F962" s="17"/>
+      <c r="F962" s="16"/>
     </row>
     <row r="963" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F963" s="17"/>
+      <c r="F963" s="16"/>
     </row>
     <row r="964" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F964" s="17"/>
+      <c r="F964" s="16"/>
     </row>
     <row r="965" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F965" s="17"/>
+      <c r="F965" s="16"/>
     </row>
     <row r="966" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F966" s="17"/>
+      <c r="F966" s="16"/>
     </row>
     <row r="967" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F967" s="17"/>
+      <c r="F967" s="16"/>
     </row>
     <row r="968" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F968" s="17"/>
+      <c r="F968" s="16"/>
     </row>
     <row r="969" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F969" s="17"/>
+      <c r="F969" s="16"/>
     </row>
     <row r="970" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F970" s="17"/>
+      <c r="F970" s="16"/>
     </row>
     <row r="971" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F971" s="17"/>
+      <c r="F971" s="16"/>
     </row>
     <row r="972" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F972" s="17"/>
+      <c r="F972" s="16"/>
     </row>
     <row r="973" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F973" s="17"/>
+      <c r="F973" s="16"/>
     </row>
     <row r="974" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F974" s="17"/>
+      <c r="F974" s="16"/>
     </row>
     <row r="975" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F975" s="17"/>
+      <c r="F975" s="16"/>
     </row>
     <row r="976" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F976" s="17"/>
+      <c r="F976" s="16"/>
     </row>
     <row r="977" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F977" s="17"/>
+      <c r="F977" s="16"/>
     </row>
     <row r="978" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F978" s="17"/>
+      <c r="F978" s="16"/>
     </row>
     <row r="979" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F979" s="17"/>
+      <c r="F979" s="16"/>
     </row>
     <row r="980" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F980" s="17"/>
+      <c r="F980" s="16"/>
     </row>
     <row r="981" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F981" s="17"/>
+      <c r="F981" s="16"/>
     </row>
     <row r="982" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F982" s="17"/>
+      <c r="F982" s="16"/>
     </row>
     <row r="983" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F983" s="17"/>
+      <c r="F983" s="16"/>
     </row>
     <row r="984" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F984" s="17"/>
+      <c r="F984" s="16"/>
     </row>
     <row r="985" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F985" s="17"/>
+      <c r="F985" s="16"/>
     </row>
     <row r="986" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F986" s="17"/>
+      <c r="F986" s="16"/>
     </row>
     <row r="987" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F987" s="17"/>
+      <c r="F987" s="16"/>
     </row>
     <row r="988" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F988" s="17"/>
+      <c r="F988" s="16"/>
     </row>
     <row r="989" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F989" s="17"/>
+      <c r="F989" s="16"/>
     </row>
     <row r="990" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F990" s="17"/>
+      <c r="F990" s="16"/>
     </row>
     <row r="991" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F991" s="17"/>
+      <c r="F991" s="16"/>
     </row>
     <row r="992" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F992" s="17"/>
+      <c r="F992" s="16"/>
     </row>
     <row r="993" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F993" s="17"/>
+      <c r="F993" s="16"/>
     </row>
     <row r="994" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F994" s="17"/>
+      <c r="F994" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
new query files and notebook updates
</commit_message>
<xml_diff>
--- a/working_files/Pathway Evidence type.xlsx
+++ b/working_files/Pathway Evidence type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Documents\GitHub\knetgraphs-gene-traits\working_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307A682C-06A7-4EF5-B0F1-A72C5F435A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F895A0-1F47-4287-BE11-8ADD0EC70CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
-  <si>
-    <t>Pathway</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Evidence Type</t>
   </si>
@@ -188,17 +185,57 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Trait Pathway</t>
+  </si>
+  <si>
+    <t>BioProc Pathway</t>
+  </si>
+  <si>
+    <t>(:Gene) - [:part_of] -&gt; (:CoExpCluster) - [:enriched_for] -&gt; (:BioProc)</t>
+  </si>
+  <si>
+    <t>(:Gene) - [:participates_in] -&gt; (:BioProc)</t>
+  </si>
+  <si>
+    <t>(:Gene) - [:differentially_expressed] -&gt; (:DGES) - [:enriched_for] -&gt; (:BioProc)</t>
+  </si>
+  <si>
+    <t>(:Gene) - [:enc] -&gt; (:Protein) - [:h_s_s|ortho|xref*0..1] - (:Protein) - [:participates_in] -&gt; (:BioProc)</t>
+  </si>
+  <si>
+    <t>(:Gene) - [:enc] -&gt; (:Protein) - [:h_s_s|ortho|xref*0..1] - (:Protein) - [:has_domain] -&gt; (:ProtDomain) - [:participates_in] -&gt; (:BioProc)</t>
+  </si>
+  <si>
+    <t>(:Gene) - [:enc] -&gt; (:Protein) - [:ortho] - (:Protein) &lt;- [:enc] - (:Gene) - [:participates_in] -&gt; (:BioProc)</t>
+  </si>
+  <si>
+    <t>(:Gene) - [:homoeolog] - (:Gene) - [:participates_in] -&gt; (:BioProc)</t>
+  </si>
+  <si>
+    <t>(:Gene) - [:regulates|genetic|physical] - (:Gene) - [:participates_in] -&gt; (:BioProc)</t>
+  </si>
+  <si>
+    <t>(:Gene) - [:enc] -&gt; (:Protein) - [:ortho] - (:Protein) &lt;- [:enc] - (:Gene) - [:genetic|physical] - (:Gene) - [:participates_in] -&gt; (:BioProc)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -293,53 +330,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,17 +593,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K994"/>
+  <dimension ref="A1:K995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="157.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="153.28515625" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
@@ -579,54 +617,54 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="7">
         <v>8737</v>
@@ -649,19 +687,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="10">
-        <v>0</v>
-      </c>
-      <c r="D3" s="10">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="F3" s="11">
         <v>0</v>
@@ -684,19 +722,19 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>19</v>
       </c>
       <c r="F4" s="32">
         <v>2339</v>
@@ -719,10 +757,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C5" s="6">
         <v>1</v>
@@ -731,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="7">
         <v>14732</v>
@@ -754,10 +792,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -766,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="7">
         <v>290458</v>
@@ -789,10 +827,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -801,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="14">
         <v>0</v>
@@ -824,10 +862,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -836,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="14">
         <v>0</v>
@@ -859,10 +897,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="10">
         <v>1</v>
@@ -871,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="11">
         <v>0</v>
@@ -894,10 +932,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -906,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="7">
         <v>4239</v>
@@ -929,10 +967,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="10">
         <v>0</v>
@@ -941,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="11">
         <v>0</v>
@@ -964,10 +1002,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6">
         <v>0</v>
@@ -976,7 +1014,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="7">
         <v>81001</v>
@@ -999,10 +1037,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="10">
         <v>0</v>
@@ -1011,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="11">
         <v>0</v>
@@ -1034,10 +1072,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="6">
         <v>0</v>
@@ -1046,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="14">
         <v>0</v>
@@ -1069,10 +1107,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="10">
         <v>0</v>
@@ -1081,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="11">
         <v>0</v>
@@ -1104,10 +1142,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
@@ -1116,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="14">
         <v>0</v>
@@ -1139,10 +1177,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
@@ -1151,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="7">
         <v>8004</v>
@@ -1174,10 +1212,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="10">
         <v>1</v>
@@ -1186,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="11">
         <v>0</v>
@@ -1209,10 +1247,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="6">
         <v>1</v>
@@ -1221,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19" s="14">
         <v>0</v>
@@ -1244,10 +1282,10 @@
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
@@ -1256,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" s="7">
         <v>93236</v>
@@ -1279,10 +1317,10 @@
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
@@ -1291,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F21" s="7">
         <v>9144</v>
@@ -1314,10 +1352,10 @@
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
@@ -1326,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" s="7">
         <v>183203</v>
@@ -1349,10 +1387,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -1361,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="7">
         <v>224667</v>
@@ -1384,10 +1422,10 @@
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
@@ -1396,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="7">
         <v>5027</v>
@@ -1419,10 +1457,10 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
@@ -1431,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" s="7">
         <v>215406</v>
@@ -1457,7 +1495,7 @@
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -1517,73 +1555,146 @@
       <c r="F31" s="25"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
+      <c r="A32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="F32" s="25"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
+      <c r="C33" s="24">
+        <v>0</v>
+      </c>
+      <c r="D33" s="24">
+        <v>0</v>
+      </c>
       <c r="E33" s="24"/>
       <c r="F33" s="25"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
+      <c r="C34" s="24">
+        <v>0</v>
+      </c>
+      <c r="D34" s="24">
+        <v>0</v>
+      </c>
       <c r="E34" s="24"/>
       <c r="F34" s="25"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
+      <c r="C35" s="24">
+        <v>0</v>
+      </c>
+      <c r="D35" s="24">
+        <v>0</v>
+      </c>
       <c r="E35" s="24"/>
       <c r="F35" s="25"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
+      <c r="C36" s="24">
+        <v>1</v>
+      </c>
+      <c r="D36" s="24">
+        <v>0</v>
+      </c>
       <c r="E36" s="24"/>
       <c r="F36" s="25"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="34" t="s">
+        <v>59</v>
+      </c>
       <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
+      <c r="C37" s="24">
+        <v>0</v>
+      </c>
+      <c r="D37" s="24">
+        <v>1</v>
+      </c>
       <c r="E37" s="24"/>
       <c r="F37" s="25"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
+      <c r="C38" s="24">
+        <v>1</v>
+      </c>
+      <c r="D38" s="24">
+        <v>0</v>
+      </c>
       <c r="E38" s="24"/>
       <c r="F38" s="25"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
+      <c r="C39" s="24">
+        <v>1</v>
+      </c>
+      <c r="D39" s="24">
+        <v>0</v>
+      </c>
       <c r="E39" s="24"/>
       <c r="F39" s="25"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
+      <c r="C40" s="24">
+        <v>1</v>
+      </c>
+      <c r="D40" s="24">
+        <v>0</v>
+      </c>
       <c r="E40" s="24"/>
       <c r="F40" s="25"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="24"/>
+      <c r="A41" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24">
+        <v>1</v>
+      </c>
+      <c r="D41" s="24">
+        <v>1</v>
+      </c>
       <c r="E41" s="24"/>
       <c r="F41" s="25"/>
     </row>
@@ -1596,24 +1707,24 @@
       <c r="F42" s="25"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="24"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="25"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="27"/>
-      <c r="C44" s="28"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="27"/>
-      <c r="E44" s="26"/>
+      <c r="E44" s="27"/>
       <c r="F44" s="24"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="29"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="28"/>
       <c r="D45" s="27"/>
       <c r="E45" s="26"/>
@@ -1621,10 +1732,10 @@
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="27"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="28"/>
       <c r="D46" s="27"/>
-      <c r="E46" s="30"/>
+      <c r="E46" s="26"/>
       <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1638,7 +1749,7 @@
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
       <c r="B48" s="27"/>
-      <c r="C48" s="31"/>
+      <c r="C48" s="28"/>
       <c r="D48" s="27"/>
       <c r="E48" s="30"/>
       <c r="F48" s="24"/>
@@ -1648,15 +1759,15 @@
       <c r="B49" s="27"/>
       <c r="C49" s="31"/>
       <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
+      <c r="E49" s="30"/>
       <c r="F49" s="24"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
       <c r="B50" s="27"/>
-      <c r="C50" s="28"/>
+      <c r="C50" s="31"/>
       <c r="D50" s="27"/>
-      <c r="E50" s="30"/>
+      <c r="E50" s="27"/>
       <c r="F50" s="24"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1664,15 +1775,15 @@
       <c r="B51" s="27"/>
       <c r="C51" s="28"/>
       <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
+      <c r="E51" s="30"/>
       <c r="F51" s="24"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22"/>
       <c r="B52" s="27"/>
-      <c r="C52" s="31"/>
+      <c r="C52" s="28"/>
       <c r="D52" s="27"/>
-      <c r="E52" s="30"/>
+      <c r="E52" s="27"/>
       <c r="F52" s="24"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1680,21 +1791,21 @@
       <c r="B53" s="27"/>
       <c r="C53" s="31"/>
       <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
+      <c r="E53" s="30"/>
       <c r="F53" s="24"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22"/>
       <c r="B54" s="27"/>
-      <c r="C54" s="28"/>
+      <c r="C54" s="31"/>
       <c r="D54" s="27"/>
-      <c r="E54" s="30"/>
+      <c r="E54" s="27"/>
       <c r="F54" s="24"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
       <c r="B55" s="27"/>
-      <c r="C55" s="31"/>
+      <c r="C55" s="28"/>
       <c r="D55" s="27"/>
       <c r="E55" s="30"/>
       <c r="F55" s="24"/>
@@ -1702,7 +1813,7 @@
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22"/>
       <c r="B56" s="27"/>
-      <c r="C56" s="28"/>
+      <c r="C56" s="31"/>
       <c r="D56" s="27"/>
       <c r="E56" s="30"/>
       <c r="F56" s="24"/>
@@ -1720,7 +1831,7 @@
       <c r="B58" s="27"/>
       <c r="C58" s="28"/>
       <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
+      <c r="E58" s="30"/>
       <c r="F58" s="24"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1728,11 +1839,11 @@
       <c r="B59" s="27"/>
       <c r="C59" s="28"/>
       <c r="D59" s="27"/>
-      <c r="E59" s="30"/>
+      <c r="E59" s="27"/>
       <c r="F59" s="24"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
+      <c r="A60" s="22"/>
       <c r="B60" s="27"/>
       <c r="C60" s="28"/>
       <c r="D60" s="27"/>
@@ -1744,139 +1855,140 @@
       <c r="B61" s="27"/>
       <c r="C61" s="28"/>
       <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
+      <c r="E61" s="30"/>
       <c r="F61" s="24"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
       <c r="F62" s="24"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="21"/>
-      <c r="B63" s="30"/>
+      <c r="A63" s="23"/>
+      <c r="B63" s="26"/>
       <c r="C63" s="30"/>
-      <c r="D63" s="27"/>
+      <c r="D63" s="26"/>
       <c r="E63" s="26"/>
       <c r="F63" s="24"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="26"/>
+      <c r="A64" s="21"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="27"/>
       <c r="E64" s="26"/>
-      <c r="F64" s="25"/>
-    </row>
-    <row r="65" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="24"/>
+      <c r="F64" s="24"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="26"/>
       <c r="D65" s="26"/>
       <c r="E65" s="26"/>
       <c r="F65" s="25"/>
     </row>
-    <row r="66" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="24"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
       <c r="F66" s="25"/>
     </row>
-    <row r="67" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="24"/>
       <c r="C67" s="24"/>
       <c r="D67" s="24"/>
       <c r="E67" s="24"/>
       <c r="F67" s="25"/>
     </row>
-    <row r="68" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="24"/>
       <c r="C68" s="24"/>
       <c r="D68" s="24"/>
       <c r="E68" s="24"/>
       <c r="F68" s="25"/>
     </row>
-    <row r="69" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="24"/>
       <c r="C69" s="24"/>
       <c r="D69" s="24"/>
       <c r="E69" s="24"/>
       <c r="F69" s="25"/>
     </row>
-    <row r="70" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="24"/>
       <c r="C70" s="24"/>
       <c r="D70" s="24"/>
       <c r="E70" s="24"/>
       <c r="F70" s="25"/>
     </row>
-    <row r="71" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="24"/>
       <c r="C71" s="24"/>
       <c r="D71" s="24"/>
       <c r="E71" s="24"/>
       <c r="F71" s="25"/>
     </row>
-    <row r="72" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="24"/>
       <c r="C72" s="24"/>
       <c r="D72" s="24"/>
       <c r="E72" s="24"/>
       <c r="F72" s="25"/>
     </row>
-    <row r="73" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="24"/>
       <c r="C73" s="24"/>
       <c r="D73" s="24"/>
       <c r="E73" s="24"/>
       <c r="F73" s="25"/>
     </row>
-    <row r="74" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="24"/>
       <c r="C74" s="24"/>
       <c r="D74" s="24"/>
       <c r="E74" s="24"/>
       <c r="F74" s="25"/>
     </row>
-    <row r="75" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="24"/>
       <c r="C75" s="24"/>
       <c r="D75" s="24"/>
       <c r="E75" s="24"/>
       <c r="F75" s="25"/>
     </row>
-    <row r="76" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="24"/>
       <c r="C76" s="24"/>
       <c r="D76" s="24"/>
       <c r="E76" s="24"/>
       <c r="F76" s="25"/>
     </row>
-    <row r="77" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="24"/>
       <c r="C77" s="24"/>
       <c r="D77" s="24"/>
       <c r="E77" s="24"/>
       <c r="F77" s="25"/>
     </row>
-    <row r="78" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="24"/>
       <c r="C78" s="24"/>
       <c r="D78" s="24"/>
       <c r="E78" s="24"/>
       <c r="F78" s="25"/>
     </row>
-    <row r="79" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="24"/>
       <c r="C79" s="24"/>
       <c r="D79" s="24"/>
       <c r="E79" s="24"/>
       <c r="F79" s="25"/>
     </row>
-    <row r="80" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
       <c r="D80" s="24"/>
@@ -1982,7 +2094,11 @@
       <c r="F94" s="25"/>
     </row>
     <row r="95" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F95" s="16"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="25"/>
     </row>
     <row r="96" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F96" s="16"/>
@@ -4681,8 +4797,11 @@
     <row r="994" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F994" s="16"/>
     </row>
+    <row r="995" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F995" s="16"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>